<commit_message>
updating bedload stuff for supporting material
</commit_message>
<xml_diff>
--- a/data/bedload_tauc/Wilcock2002_tauc.xlsx
+++ b/data/bedload_tauc/Wilcock2002_tauc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Shear Stress\bedload_tauc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data\bedload_tauc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A66BE3-DD0B-48AC-BEE7-DB7CC6DD94A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E241641-2121-416E-BF3A-DBF1FAD1AD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12555" yWindow="330" windowWidth="12480" windowHeight="15150" activeTab="2" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
   </bookViews>
   <sheets>
     <sheet name="Dg-Ds Calculation" sheetId="2" r:id="rId1"/>
@@ -464,6 +464,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -480,13 +487,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7413,7 +7413,7 @@
   <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7426,18 +7426,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="42"/>
+      <c r="C2" s="45"/>
       <c r="H2" s="18" t="s">
         <v>16</v>
       </c>
@@ -7736,12 +7736,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H14" s="44" t="s">
+      <c r="H14" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="24">
@@ -8176,10 +8176,10 @@
       <c r="F1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="45"/>
+      <c r="I1" s="48"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8208,11 +8208,11 @@
         <f>$I$20+($I$19-$I$20)*EXP(-14*A2)</f>
         <v>1.3290468742698638</v>
       </c>
-      <c r="H2" s="45" t="str">
+      <c r="H2" s="48" t="str">
         <f>B1</f>
         <v>Tri* (Dg/Ds = 10)</v>
       </c>
-      <c r="I2" s="45"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8340,11 +8340,11 @@
         <f t="shared" si="4"/>
         <v>0.7870350317127095</v>
       </c>
-      <c r="H6" s="45" t="str">
+      <c r="H6" s="48" t="str">
         <f>C1</f>
         <v>Tri* (Dg/Ds = 20)</v>
       </c>
-      <c r="I6" s="45"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -8472,11 +8472,11 @@
         <f t="shared" si="4"/>
         <v>0.4774329545306662</v>
       </c>
-      <c r="H10" s="45" t="str">
+      <c r="H10" s="48" t="str">
         <f>D1</f>
         <v>Tri* (Dg/Ds = 35)</v>
       </c>
-      <c r="I10" s="45"/>
+      <c r="I10" s="48"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -8604,11 +8604,11 @@
         <f t="shared" si="4"/>
         <v>0.30058544185786273</v>
       </c>
-      <c r="H14" s="45" t="str">
+      <c r="H14" s="48" t="str">
         <f>E1</f>
         <v>Tri* (Dg/Ds = 50)</v>
       </c>
-      <c r="I14" s="45"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -8733,11 +8733,11 @@
         <f t="shared" si="4"/>
         <v>0.1995685397000391</v>
       </c>
-      <c r="H18" s="45" t="str">
+      <c r="H18" s="48" t="str">
         <f>F1</f>
         <v>Tri* (Dg/Ds = 43.4)</v>
       </c>
-      <c r="I18" s="45"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
   <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11043,13 +11043,13 @@
       <c r="B1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -11298,20 +11298,20 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="41" t="s">
         <v>43</v>
       </c>
       <c r="B16"/>
@@ -11328,7 +11328,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="48">
+      <c r="A18" s="42">
         <v>2</v>
       </c>
       <c r="B18" s="2">
@@ -11340,7 +11340,7 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="48">
+      <c r="A19" s="42">
         <v>20</v>
       </c>
       <c r="B19" s="2">
@@ -11352,11 +11352,11 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="48">
+      <c r="A20" s="42">
         <v>45</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" ref="B19:B29" si="2">$B$7*($B$11-$B$10)*$B$12*($A20/1000000)</f>
+        <f t="shared" ref="B20:B29" si="2">$B$7*($B$11-$B$10)*$B$12*($A20/1000000)</f>
         <v>0.63163795468547745</v>
       </c>
       <c r="C20" s="2"/>
@@ -11364,7 +11364,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="48">
+      <c r="A21" s="42">
         <v>63</v>
       </c>
       <c r="B21" s="2">
@@ -11376,7 +11376,7 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="49">
+      <c r="A22" s="43">
         <v>100</v>
       </c>
       <c r="B22" s="2">
@@ -11388,7 +11388,7 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="49">
+      <c r="A23" s="43">
         <v>200</v>
       </c>
       <c r="B23" s="2">
@@ -11400,7 +11400,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="49">
+      <c r="A24" s="43">
         <v>280</v>
       </c>
       <c r="B24" s="2">
@@ -11412,7 +11412,7 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="49">
+      <c r="A25" s="43">
         <v>500</v>
       </c>
       <c r="B25" s="2">
@@ -11424,7 +11424,7 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="49">
+      <c r="A26" s="43">
         <v>700</v>
       </c>
       <c r="B26" s="2">
@@ -11436,7 +11436,7 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="49">
+      <c r="A27" s="43">
         <v>850</v>
       </c>
       <c r="B27" s="2">
@@ -11448,7 +11448,7 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="49">
+      <c r="A28" s="43">
         <v>1000</v>
       </c>
       <c r="B28" s="2">
@@ -11472,7 +11472,7 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="49">
+      <c r="A30" s="43">
         <v>2000</v>
       </c>
       <c r="B30" s="2">
@@ -11491,8 +11491,13 @@
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="2">
+        <v>630</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" ref="B32" si="3">$B$7*($B$11-$B$10)*$B$12*($A32/1000000)</f>
+        <v>8.8429313655966837</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>

</xml_diff>

<commit_message>
organized the Ds calculations for fs content in bed
</commit_message>
<xml_diff>
--- a/data/bedload_tauc/Wilcock2002_tauc.xlsx
+++ b/data/bedload_tauc/Wilcock2002_tauc.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data\bedload_tauc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\sediment_trap_paper\data\bedload_tauc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E241641-2121-416E-BF3A-DBF1FAD1AD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C620D067-0743-4346-AC34-48F3412F6E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dg-Ds Calculation" sheetId="2" r:id="rId1"/>
-    <sheet name="Dimensionless Tau ri" sheetId="1" r:id="rId2"/>
-    <sheet name="Dimensional Tau ri" sheetId="3" r:id="rId3"/>
+    <sheet name="Sand GSD calculations" sheetId="4" r:id="rId1"/>
+    <sheet name="Dg-Ds Calculation" sheetId="2" r:id="rId2"/>
+    <sheet name="Dimensionless Tau ri" sheetId="1" r:id="rId3"/>
+    <sheet name="Dimensional Tau ri" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={41D31C07-9A80-4AD8-B2A3-5FDC4E7CAE5D}</author>
+    <author>tc={EFCC6145-FFA2-4349-A159-0958462C0847}</author>
+  </authors>
+  <commentList>
+    <comment ref="K30" authorId="0" shapeId="0" xr:uid="{41D31C07-9A80-4AD8-B2A3-5FDC4E7CAE5D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Instead of in the pebble count having sand content = 4.5%, we are quantifying these percentages to each sand size</t>
+      </text>
+    </comment>
+    <comment ref="I31" authorId="1" shapeId="0" xr:uid="{EFCC6145-FFA2-4349-A159-0958462C0847}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is basically saying “From the 4.5% of sand in the bed (from pebble count), 0.14% is 0.001mm; 0.97% is 0.005mm; etc...</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>Fs</t>
   </si>
@@ -77,12 +105,6 @@
   </si>
   <si>
     <t>Cum</t>
-  </si>
-  <si>
-    <t>Fines</t>
-  </si>
-  <si>
-    <t>D50</t>
   </si>
   <si>
     <t>Frequency</t>
@@ -171,6 +193,93 @@
   <si>
     <t>Dimensional Tauc by Size (um) in Pa</t>
   </si>
+  <si>
+    <t>La Jara - Full</t>
+  </si>
+  <si>
+    <t>Gravelometer Size</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>cum finer</t>
+  </si>
+  <si>
+    <t>% finer</t>
+  </si>
+  <si>
+    <t>sand &lt; 1 mm</t>
+  </si>
+  <si>
+    <t>TOTAL + SAND</t>
+  </si>
+  <si>
+    <t>% BED SAND</t>
+  </si>
+  <si>
+    <t>cum</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>LISST bed GSD &lt;500 um</t>
+  </si>
+  <si>
+    <t>Size (microns)</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting Percent Sand: </t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interpolated sand sizes from LISST </t>
+  </si>
+  <si>
+    <t>Adding these sand percentages to pebble count percentages:</t>
+  </si>
+  <si>
+    <t>% Sand Sizes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total= </t>
+  </si>
+  <si>
+    <t>Sand not considered</t>
+  </si>
+  <si>
+    <t>Sand is considered</t>
+  </si>
+  <si>
+    <t>% finer (cum)</t>
+  </si>
+  <si>
+    <t>(4.52%!)</t>
+  </si>
+  <si>
+    <t>Fines (&lt;0.05)</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">between 1 and 11 mm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINAL GSD - including sand sizes! </t>
+  </si>
 </sst>
 </file>
 
@@ -182,7 +291,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +323,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,8 +397,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -308,7 +459,20 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -319,11 +483,13 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -333,18 +499,18 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,12 +540,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -439,9 +599,6 @@
     <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,20 +618,8 @@
     <xf numFmtId="165" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -487,6 +632,120 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -618,16 +877,16 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -639,19 +898,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.22500000000000001</c:v>
+                  <c:v>0.21951219512195122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27500000000000002</c:v>
+                  <c:v>0.26829268292682928</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92500000000000004</c:v>
+                  <c:v>0.29268292682926833</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95000000000000007</c:v>
+                  <c:v>0.92682926829268297</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.95121951219512202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,6 +1188,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -936,7 +1196,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1075,7 +1334,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dg-Ds Calculation'!$H$16:$H$26</c:f>
+              <c:f>'Dg-Ds Calculation'!$H$18:$H$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1117,7 +1376,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dg-Ds Calculation'!$K$16:$K$26</c:f>
+              <c:f>'Dg-Ds Calculation'!$K$18:$K$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1430,6 +1689,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1437,7 +1697,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5122,6 +5381,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -5129,7 +5389,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6836,14 +7095,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7091,6 +7350,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Hucke Nunez, Nicole (huck4481@vandals.uidaho.edu)" id="{DEAD2044-8BC9-4EBB-969E-0C2C739F9BAD}" userId="S::huck4481@vandals.uidaho.edu::b4d3cd24-8849-4526-aedb-574e3308a974" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7408,12 +7673,1798 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K30" dT="2026-01-16T20:59:27.14" personId="{DEAD2044-8BC9-4EBB-969E-0C2C739F9BAD}" id="{41D31C07-9A80-4AD8-B2A3-5FDC4E7CAE5D}">
+    <text>Instead of in the pebble count having sand content = 4.5%, we are quantifying these percentages to each sand size</text>
+  </threadedComment>
+  <threadedComment ref="I31" dT="2026-01-16T20:58:23.68" personId="{DEAD2044-8BC9-4EBB-969E-0C2C739F9BAD}" id="{EFCC6145-FFA2-4349-A159-0958462C0847}">
+    <text>This is basically saying “From the 4.5% of sand in the bed (from pebble count), 0.14% is 0.001mm; 0.97% is 0.005mm; etc...</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529AA10A-7A72-482C-95E8-4CA51D7B8E74}">
-  <dimension ref="B1:K35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBF568F-4DC0-410C-BEDF-98C183FB2880}">
+  <dimension ref="B1:S74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J1" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="70"/>
+      <c r="J2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="10">
+        <f>SUM(L32:L39)</f>
+        <v>9.359555488395413E-3</v>
+      </c>
+      <c r="L3" s="10">
+        <f>K3</f>
+        <v>9.359555488395413E-3</v>
+      </c>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="73"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="9">
+        <v>10</v>
+      </c>
+      <c r="D4" s="46">
+        <v>0</v>
+      </c>
+      <c r="E4" s="47">
+        <f>D4/$D$18*100</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="72">
+        <f>SUM(L32:L42)</f>
+        <v>1.990567778890236E-2</v>
+      </c>
+      <c r="G4" s="68">
+        <f>F4</f>
+        <v>1.990567778890236E-2</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="12">
+        <f>L40</f>
+        <v>8.650709206137662E-3</v>
+      </c>
+      <c r="L4" s="10">
+        <f>K4+L3</f>
+        <v>1.8010264694533075E-2</v>
+      </c>
+      <c r="M4" s="74"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="73"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="55">
+        <f>L43</f>
+        <v>2.5343191042496417E-2</v>
+      </c>
+      <c r="G5" s="55">
+        <f>F5+G4</f>
+        <v>4.5248868831398781E-2</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" ref="K5:K7" si="0">L41</f>
+        <v>1.2320185113400368E-3</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" ref="L5:L22" si="1">K5+L4</f>
+        <v>1.9242283205873113E-2</v>
+      </c>
+      <c r="M5" s="74"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <f>C6+D4</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="49">
+        <f>D6/$D$18*100</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="69">
+        <f>C6/$C$19</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="55">
+        <f t="shared" ref="G6:G18" si="2">F6+G5</f>
+        <v>4.5248868831398781E-2</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="K6" s="12">
+        <f t="shared" si="0"/>
+        <v>6.6339458302924835E-4</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="1"/>
+        <v>1.990567778890236E-2</v>
+      </c>
+      <c r="M6" s="74"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="9">
+        <v>5.6</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" ref="D7:D17" si="3">C7+D6</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="49">
+        <f t="shared" ref="E7:E17" si="4">D7/$D$18*100</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="69">
+        <f t="shared" ref="F7:F18" si="5">C7/$C$19</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="55">
+        <f t="shared" si="2"/>
+        <v>4.5248868831398781E-2</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" si="0"/>
+        <v>2.5343191042496417E-2</v>
+      </c>
+      <c r="L7" s="10">
+        <f>K7+L6</f>
+        <v>4.5248868831398781E-2</v>
+      </c>
+      <c r="M7" s="74"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="50"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="69">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="55">
+        <f t="shared" si="2"/>
+        <v>4.5248868831398781E-2</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="K8" s="12">
+        <f>L8-L7</f>
+        <v>9.0497737556561458E-4</v>
+      </c>
+      <c r="L8" s="10">
+        <f>$G$21*J8+$G$22</f>
+        <v>4.6153846206964395E-2</v>
+      </c>
+      <c r="M8" s="74"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="50"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>11</v>
+      </c>
+      <c r="C9" s="9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="49">
+        <f t="shared" si="4"/>
+        <v>2.3696682464454977</v>
+      </c>
+      <c r="F9" s="69">
+        <f t="shared" si="5"/>
+        <v>2.2624434389140271E-2</v>
+      </c>
+      <c r="G9" s="55">
+        <f t="shared" si="2"/>
+        <v>6.7873303220539055E-2</v>
+      </c>
+      <c r="J9" s="11">
+        <v>2</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" ref="K9:K14" si="6">L9-L8</f>
+        <v>1.3574660633484115E-3</v>
+      </c>
+      <c r="L9" s="10">
+        <f>$G$21*J9+$G$22</f>
+        <v>4.7511312270312807E-2</v>
+      </c>
+      <c r="M9" s="74"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="50"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="E10" s="49">
+        <f t="shared" si="4"/>
+        <v>7.109004739336493</v>
+      </c>
+      <c r="F10" s="69">
+        <f t="shared" si="5"/>
+        <v>4.5248868778280542E-2</v>
+      </c>
+      <c r="G10" s="55">
+        <f t="shared" si="2"/>
+        <v>0.1131221719988196</v>
+      </c>
+      <c r="J10" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="K10" s="23">
+        <f t="shared" si="6"/>
+        <v>1.8099547511312222E-3</v>
+      </c>
+      <c r="L10" s="10">
+        <f>$G$21*J10+$G$22</f>
+        <v>4.9321267021444029E-2</v>
+      </c>
+      <c r="M10" s="74"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="50"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <v>22.6</v>
+      </c>
+      <c r="C11" s="9">
+        <v>25</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="E11" s="49">
+        <f t="shared" si="4"/>
+        <v>18.957345971563981</v>
+      </c>
+      <c r="F11" s="69">
+        <f t="shared" si="5"/>
+        <v>0.11312217194570136</v>
+      </c>
+      <c r="G11" s="55">
+        <f t="shared" si="2"/>
+        <v>0.22624434394452098</v>
+      </c>
+      <c r="J11" s="22">
+        <v>4</v>
+      </c>
+      <c r="K11" s="23">
+        <f t="shared" si="6"/>
+        <v>2.7149321266968368E-3</v>
+      </c>
+      <c r="L11" s="10">
+        <f>$G$21*J11+$G$22</f>
+        <v>5.2036199148140866E-2</v>
+      </c>
+      <c r="M11" s="74"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="50"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="51">
+        <v>32</v>
+      </c>
+      <c r="C12" s="51">
+        <v>27</v>
+      </c>
+      <c r="D12" s="51">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="E12" s="52">
+        <f t="shared" si="4"/>
+        <v>31.753554502369667</v>
+      </c>
+      <c r="F12" s="69">
+        <f t="shared" si="5"/>
+        <v>0.12217194570135746</v>
+      </c>
+      <c r="G12" s="55">
+        <f t="shared" si="2"/>
+        <v>0.34841628964587845</v>
+      </c>
+      <c r="J12" s="22">
+        <v>5.6</v>
+      </c>
+      <c r="K12" s="23">
+        <f>L12-L11</f>
+        <v>3.6199095022624445E-3</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" ref="L12:L13" si="7">$G$21*J12+$G$22</f>
+        <v>5.565610865040331E-2</v>
+      </c>
+      <c r="M12" s="74"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="50"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="51">
+        <v>45</v>
+      </c>
+      <c r="C13" s="51">
+        <v>43</v>
+      </c>
+      <c r="D13" s="51">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="E13" s="52">
+        <f t="shared" si="4"/>
+        <v>52.132701421800952</v>
+      </c>
+      <c r="F13" s="69">
+        <f t="shared" si="5"/>
+        <v>0.19457013574660634</v>
+      </c>
+      <c r="G13" s="55">
+        <f t="shared" si="2"/>
+        <v>0.54298642539248476</v>
+      </c>
+      <c r="J13" s="22">
+        <v>8</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="6"/>
+        <v>5.4298642533936597E-3</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="7"/>
+        <v>6.108597290379697E-2</v>
+      </c>
+      <c r="M13" s="74"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="50"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>64</v>
+      </c>
+      <c r="C14" s="9">
+        <v>43</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="E14" s="49">
+        <f t="shared" si="4"/>
+        <v>72.511848341232238</v>
+      </c>
+      <c r="F14" s="69">
+        <f t="shared" si="5"/>
+        <v>0.19457013574660634</v>
+      </c>
+      <c r="G14" s="55">
+        <f t="shared" si="2"/>
+        <v>0.73755656113909107</v>
+      </c>
+      <c r="J14" s="22">
+        <v>11</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="6"/>
+        <v>6.7873303167420851E-3</v>
+      </c>
+      <c r="L14" s="10">
+        <f>G9</f>
+        <v>6.7873303220539055E-2</v>
+      </c>
+      <c r="M14" s="74"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="50"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="9">
+        <v>90</v>
+      </c>
+      <c r="C15" s="9">
+        <v>35</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="E15" s="49">
+        <f t="shared" si="4"/>
+        <v>89.099526066350705</v>
+      </c>
+      <c r="F15" s="69">
+        <f t="shared" si="5"/>
+        <v>0.15837104072398189</v>
+      </c>
+      <c r="G15" s="55">
+        <f t="shared" si="2"/>
+        <v>0.89592760186307296</v>
+      </c>
+      <c r="J15" s="22">
+        <v>16</v>
+      </c>
+      <c r="K15" s="23">
+        <f>F10</f>
+        <v>4.5248868778280542E-2</v>
+      </c>
+      <c r="L15" s="10">
+        <f>K15+L14</f>
+        <v>0.1131221719988196</v>
+      </c>
+      <c r="M15" s="74"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="50"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>128</v>
+      </c>
+      <c r="C16" s="9">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="E16" s="49">
+        <f t="shared" si="4"/>
+        <v>93.838862559241704</v>
+      </c>
+      <c r="F16" s="69">
+        <f t="shared" si="5"/>
+        <v>4.5248868778280542E-2</v>
+      </c>
+      <c r="G16" s="55">
+        <f t="shared" si="2"/>
+        <v>0.94117647064135346</v>
+      </c>
+      <c r="J16" s="22">
+        <v>22.6</v>
+      </c>
+      <c r="K16" s="23">
+        <f>F11</f>
+        <v>0.11312217194570136</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" ref="L16:L22" si="8">K16+L15</f>
+        <v>0.22624434394452098</v>
+      </c>
+      <c r="M16" s="74"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="50"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>180</v>
+      </c>
+      <c r="C17" s="9">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="3"/>
+        <v>211</v>
+      </c>
+      <c r="E17" s="49">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="F17" s="69">
+        <f t="shared" si="5"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="G17" s="55">
+        <f t="shared" si="2"/>
+        <v>1.0000000000531182</v>
+      </c>
+      <c r="J17" s="22">
+        <v>32</v>
+      </c>
+      <c r="K17" s="23">
+        <f>F12</f>
+        <v>0.12217194570135746</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="8"/>
+        <v>0.34841628964587845</v>
+      </c>
+      <c r="M17" s="74"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="50"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="9">
+        <v>211</v>
+      </c>
+      <c r="D18" s="9">
+        <v>211</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="69">
+        <f>SUM(F4:F17)</f>
+        <v>1.0000000000531182</v>
+      </c>
+      <c r="G18" s="55"/>
+      <c r="J18" s="22">
+        <v>45</v>
+      </c>
+      <c r="K18" s="23">
+        <f>F13</f>
+        <v>0.19457013574660634</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="8"/>
+        <v>0.54298642539248476</v>
+      </c>
+      <c r="M18" s="74"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
+      <c r="S18" s="50"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1">
+        <f>C18+C4</f>
+        <v>221</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="J19" s="22">
+        <v>64</v>
+      </c>
+      <c r="K19" s="23">
+        <f>F14</f>
+        <v>0.19457013574660634</v>
+      </c>
+      <c r="L19" s="10">
+        <f t="shared" si="8"/>
+        <v>0.73755656113909107</v>
+      </c>
+      <c r="M19" s="74"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="74"/>
+      <c r="S19" s="50"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="65">
+        <f>C4/C19*100</f>
+        <v>4.5248868778280542</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="J20" s="9">
+        <v>90</v>
+      </c>
+      <c r="K20" s="10">
+        <f>F15</f>
+        <v>0.15837104072398189</v>
+      </c>
+      <c r="L20" s="10">
+        <f t="shared" si="8"/>
+        <v>0.89592760186307296</v>
+      </c>
+      <c r="M20" s="74"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="74"/>
+      <c r="S20" s="50"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="67">
+        <f>(G5-G9)/(B5-B9)</f>
+        <v>2.2624434389140274E-3</v>
+      </c>
+      <c r="J21" s="9">
+        <v>128</v>
+      </c>
+      <c r="K21" s="10">
+        <f>F16</f>
+        <v>4.5248868778280542E-2</v>
+      </c>
+      <c r="L21" s="10">
+        <f t="shared" si="8"/>
+        <v>0.94117647064135346</v>
+      </c>
+      <c r="M21" s="74"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="74"/>
+      <c r="R21" s="74"/>
+      <c r="S21" s="50"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="2">
+        <f>-(G21*B5)+G5</f>
+        <v>4.2986425392484755E-2</v>
+      </c>
+      <c r="J22" s="9">
+        <v>180</v>
+      </c>
+      <c r="K22" s="10">
+        <f>F17</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="L22" s="10">
+        <f t="shared" si="8"/>
+        <v>1.0000000000531182</v>
+      </c>
+      <c r="M22" s="74"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="50"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="N23" s="1"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="50"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="53">
+        <v>0.37</v>
+      </c>
+      <c r="C24" s="3">
+        <f>D24</f>
+        <v>1.4521943478260869E-2</v>
+      </c>
+      <c r="D24" s="54">
+        <v>1.4521943478260869E-2</v>
+      </c>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="50"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="53">
+        <v>0.44</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" ref="C25:C73" si="9">D25+C24</f>
+        <v>2.9906226086956519E-2</v>
+      </c>
+      <c r="D25" s="54">
+        <v>1.5384282608695652E-2</v>
+      </c>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="50"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="53">
+        <v>0.52</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="9"/>
+        <v>4.6655078260869565E-2</v>
+      </c>
+      <c r="D26" s="54">
+        <v>1.6748852173913042E-2</v>
+      </c>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="76"/>
+      <c r="S26" s="50"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="53">
+        <v>0.61</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="9"/>
+        <v>6.5399752173913042E-2</v>
+      </c>
+      <c r="D27" s="54">
+        <v>1.8744673913043474E-2</v>
+      </c>
+      <c r="P27" s="76"/>
+      <c r="Q27" s="76"/>
+      <c r="R27" s="76"/>
+      <c r="S27" s="76"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="53">
+        <v>0.72</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="9"/>
+        <v>8.6922495652173914E-2</v>
+      </c>
+      <c r="D28" s="54">
+        <v>2.1522743478260869E-2</v>
+      </c>
+      <c r="P28" s="76"/>
+      <c r="Q28" s="76"/>
+      <c r="R28" s="76"/>
+      <c r="S28" s="76"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="53">
+        <v>0.85</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11223754782608694</v>
+      </c>
+      <c r="D29" s="54">
+        <v>2.5315052173913034E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="53">
+        <v>1.01</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="9"/>
+        <v>0.14369522173913041</v>
+      </c>
+      <c r="D30" s="54">
+        <v>3.1457673913043473E-2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="53">
+        <v>1.19</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="9"/>
+        <v>0.18734088260869564</v>
+      </c>
+      <c r="D31" s="54">
+        <v>4.3645660869565228E-2</v>
+      </c>
+      <c r="F31" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K31" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="53">
+        <v>1.4</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="9"/>
+        <v>0.25067402608695649</v>
+      </c>
+      <c r="D32" s="54">
+        <v>6.333314347826087E-2</v>
+      </c>
+      <c r="F32" s="59">
+        <v>1</v>
+      </c>
+      <c r="G32" s="63">
+        <f>1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="H32" s="49">
+        <f>C30</f>
+        <v>0.14369522173913041</v>
+      </c>
+      <c r="I32" s="3">
+        <f>H32</f>
+        <v>0.14369522173913041</v>
+      </c>
+      <c r="K32" s="63">
+        <f>1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="L32" s="66">
+        <f>I32*$C$20/10000</f>
+        <v>6.5020462325398381E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="53">
+        <v>1.65</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="9"/>
+        <v>0.329392652173913</v>
+      </c>
+      <c r="D33" s="54">
+        <v>7.8718626086956511E-2</v>
+      </c>
+      <c r="F33" s="59">
+        <v>5</v>
+      </c>
+      <c r="G33" s="63">
+        <f>5/1000</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H33" s="49">
+        <f>C39 + (F33 - B39) * ((C40 - C39) / (B40 - B39))</f>
+        <v>1.1092679565217392</v>
+      </c>
+      <c r="I33" s="3">
+        <f>H33-H32</f>
+        <v>0.96557273478260874</v>
+      </c>
+      <c r="K33" s="63">
+        <f>5/1000</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L33" s="66">
+        <f t="shared" ref="L33:L43" si="10">I33*$C$20/10000</f>
+        <v>4.3691073972063743E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="53">
+        <v>1.95</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="9"/>
+        <v>0.42033431739130428</v>
+      </c>
+      <c r="D34" s="54">
+        <v>9.094166521739129E-2</v>
+      </c>
+      <c r="F34" s="59">
+        <v>10</v>
+      </c>
+      <c r="G34" s="63">
+        <f>10/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="H34" s="49">
+        <f>C43 + (F34 - B43) * ((C44 - C43) / (B44 - B43))</f>
+        <v>1.8372186405518396</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" ref="I34:I42" si="11">H34-H33</f>
+        <v>0.72795068403010044</v>
+      </c>
+      <c r="K34" s="63">
+        <f>10/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="L34" s="66">
+        <f t="shared" si="10"/>
+        <v>3.2938944978737577E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="53">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="9"/>
+        <v>0.52298628260869562</v>
+      </c>
+      <c r="D35" s="54">
+        <v>0.10265196521739132</v>
+      </c>
+      <c r="F35" s="59">
+        <v>50</v>
+      </c>
+      <c r="G35" s="63">
+        <f>50/1000</f>
+        <v>0.05</v>
+      </c>
+      <c r="H35" s="49">
+        <f>C54 + (F35 - B54) * ((C55 - C54) / (B55 - B54))</f>
+        <v>5.8736056187979546</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="11"/>
+        <v>4.0363869782461155</v>
+      </c>
+      <c r="K35" s="63">
+        <f>50/1000</f>
+        <v>0.05</v>
+      </c>
+      <c r="L35" s="66">
+        <f t="shared" si="10"/>
+        <v>1.8264194471701882E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="53">
+        <v>2.72</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="9"/>
+        <v>0.63402316086956523</v>
+      </c>
+      <c r="D36" s="54">
+        <v>0.11103687826086958</v>
+      </c>
+      <c r="F36" s="59">
+        <v>100</v>
+      </c>
+      <c r="G36" s="63">
+        <f>100/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="49">
+        <f>C58 + (F36 - B58) * ((C59 - C58) / (B59 - B58))</f>
+        <v>7.8173612272789699</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="11"/>
+        <v>1.9437556084810153</v>
+      </c>
+      <c r="K36" s="63">
+        <f>100/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="L36" s="66">
+        <f t="shared" si="10"/>
+        <v>8.7952742465204319E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="53">
+        <v>3.2</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="9"/>
+        <v>0.75186232608695658</v>
+      </c>
+      <c r="D37" s="54">
+        <v>0.11783916521739132</v>
+      </c>
+      <c r="F37" s="59">
+        <v>200</v>
+      </c>
+      <c r="G37" s="63">
+        <f>200/1000</f>
+        <v>0.2</v>
+      </c>
+      <c r="H37" s="49">
+        <f>C63 + (F37 - B63) * ((C64 - C63) / (B64 - B63))</f>
+        <v>8.6178874743593035</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="11"/>
+        <v>0.8005262470803336</v>
+      </c>
+      <c r="K37" s="63">
+        <f>200/1000</f>
+        <v>0.2</v>
+      </c>
+      <c r="L37" s="66">
+        <f t="shared" si="10"/>
+        <v>3.6222907107707401E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="53">
+        <v>3.78</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="9"/>
+        <v>0.87711632608695655</v>
+      </c>
+      <c r="D38" s="54">
+        <v>0.125254</v>
+      </c>
+      <c r="F38" s="59">
+        <v>300</v>
+      </c>
+      <c r="G38" s="63">
+        <f>300/1000</f>
+        <v>0.3</v>
+      </c>
+      <c r="H38" s="49">
+        <f>C67 + (F38 - B67) * ((C68 - C67) / (B68 - B67))</f>
+        <v>10.45890106956522</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="11"/>
+        <v>1.8410135952059168</v>
+      </c>
+      <c r="K38" s="63">
+        <f>300/1000</f>
+        <v>0.3</v>
+      </c>
+      <c r="L38" s="66">
+        <f t="shared" si="10"/>
+        <v>8.330378258850303E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="53">
+        <v>4.46</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="9"/>
+        <v>1.0122908956521739</v>
+      </c>
+      <c r="D39" s="54">
+        <v>0.1351745695652174</v>
+      </c>
+      <c r="F39" s="59">
+        <v>400</v>
+      </c>
+      <c r="G39" s="63">
+        <v>0.4</v>
+      </c>
+      <c r="H39" s="49">
+        <f>C70 + (F39 - B70) * ((C71 - C70) / (B71 - B70))</f>
+        <v>20.684617629353859</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="11"/>
+        <v>10.225716559788639</v>
+      </c>
+      <c r="K39" s="63">
+        <v>0.4</v>
+      </c>
+      <c r="L39" s="66">
+        <f t="shared" si="10"/>
+        <v>4.6270210677776648E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="53">
+        <v>5.27</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="9"/>
+        <v>1.1577564869565218</v>
+      </c>
+      <c r="D40" s="54">
+        <v>0.1454655913043478</v>
+      </c>
+      <c r="F40" s="59">
+        <v>500</v>
+      </c>
+      <c r="G40" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="H40" s="49">
+        <f>C71 + (F40 - B71) * ((C72 - C71) / (B72 - B71))</f>
+        <v>39.802684974918094</v>
+      </c>
+      <c r="I40" s="3">
+        <f>H40-H39</f>
+        <v>19.118067345564235</v>
+      </c>
+      <c r="K40" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="L40" s="66">
+        <f t="shared" si="10"/>
+        <v>8.650709206137662E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="53">
+        <v>6.21</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="9"/>
+        <v>1.3145914695652174</v>
+      </c>
+      <c r="D41" s="54">
+        <v>0.15683498260869566</v>
+      </c>
+      <c r="F41" s="59">
+        <v>630</v>
+      </c>
+      <c r="G41" s="63">
+        <v>0.63</v>
+      </c>
+      <c r="H41" s="49">
+        <f>C71 + (F41 - B71) * ((C72 - C71) / (B72 - B71))</f>
+        <v>42.525445884979575</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" ref="I41:I43" si="12">H41-H40</f>
+        <v>2.7227609100614814</v>
+      </c>
+      <c r="K41" s="63">
+        <v>0.63</v>
+      </c>
+      <c r="L41" s="66">
+        <f t="shared" si="10"/>
+        <v>1.2320185113400368E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="53">
+        <v>7.33</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="9"/>
+        <v>1.4834078391304348</v>
+      </c>
+      <c r="D42" s="54">
+        <v>0.16881636956521742</v>
+      </c>
+      <c r="F42" s="59">
+        <v>700</v>
+      </c>
+      <c r="G42" s="63">
+        <v>0.7</v>
+      </c>
+      <c r="H42" s="49">
+        <f>C71 + (F42 - B71) * ((C72 - C71) / (B72 - B71))</f>
+        <v>43.991547913474214</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="12"/>
+        <v>1.4661020284946389</v>
+      </c>
+      <c r="K42" s="63">
+        <v>0.7</v>
+      </c>
+      <c r="L42" s="66">
+        <f t="shared" si="10"/>
+        <v>6.6339458302924835E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="53">
+        <v>8.65</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="9"/>
+        <v>1.6652984695652175</v>
+      </c>
+      <c r="D43" s="54">
+        <v>0.18189063043478262</v>
+      </c>
+      <c r="F43" s="59">
+        <v>1000</v>
+      </c>
+      <c r="G43" s="63">
+        <v>1</v>
+      </c>
+      <c r="H43" s="49">
+        <f>C72 + (F43 - B72) * ((C73 - C72) / (B73 - B72))</f>
+        <v>100.00000011739129</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="12"/>
+        <v>56.008452203917081</v>
+      </c>
+      <c r="K43" s="63">
+        <v>1</v>
+      </c>
+      <c r="L43" s="66">
+        <f t="shared" si="10"/>
+        <v>2.5343191042496417E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="53">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="9"/>
+        <v>1.8639617782608697</v>
+      </c>
+      <c r="D44" s="54">
+        <v>0.19866330869565213</v>
+      </c>
+      <c r="G44" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L44" s="67">
+        <f>SUM(L32:L43)</f>
+        <v>4.5248868831398781E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="53">
+        <v>12.05</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="9"/>
+        <v>2.0826345956521739</v>
+      </c>
+      <c r="D45" s="54">
+        <v>0.21867281739130434</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="53">
+        <v>14.22</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="9"/>
+        <v>2.3316030086956521</v>
+      </c>
+      <c r="D46" s="54">
+        <v>0.24896841304347825</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="53">
+        <v>16.78</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="9"/>
+        <v>2.6197704260869563</v>
+      </c>
+      <c r="D47" s="54">
+        <v>0.28816741739130436</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="53">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="9"/>
+        <v>2.9570251782608694</v>
+      </c>
+      <c r="D48" s="54">
+        <v>0.33725475217391304</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="53">
+        <v>23.37</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="9"/>
+        <v>3.1096920391304348</v>
+      </c>
+      <c r="D49" s="54">
+        <v>0.15266686086956519</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="53">
+        <v>25</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="9"/>
+        <v>3.3513365173913043</v>
+      </c>
+      <c r="D50" s="54">
+        <v>0.24164447826086954</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="53">
+        <v>27.58</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="9"/>
+        <v>3.8141872173913045</v>
+      </c>
+      <c r="D51" s="54">
+        <v>0.46285069999999995</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="53">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="9"/>
+        <v>4.3410367260869567</v>
+      </c>
+      <c r="D52" s="54">
+        <v>0.52684950869565228</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="53">
+        <v>38.409999999999997</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="9"/>
+        <v>4.920636043478261</v>
+      </c>
+      <c r="D53" s="54">
+        <v>0.57959931739130444</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="53">
+        <v>45.32</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="9"/>
+        <v>5.5320725695652175</v>
+      </c>
+      <c r="D54" s="54">
+        <v>0.61143652608695653</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="53">
+        <v>53.48</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="9"/>
+        <v>6.1275660913043479</v>
+      </c>
+      <c r="D55" s="54">
+        <v>0.5954935217391305</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="53">
+        <v>63.11</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="9"/>
+        <v>6.6892284173913046</v>
+      </c>
+      <c r="D56" s="54">
+        <v>0.56166232608695643</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="53">
+        <v>74.48</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="9"/>
+        <v>7.172364091304348</v>
+      </c>
+      <c r="D57" s="54">
+        <v>0.48313567391304357</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="53">
+        <v>87.89</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="9"/>
+        <v>7.5740880043478267</v>
+      </c>
+      <c r="D58" s="54">
+        <v>0.40172391304347826</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="53">
+        <v>103.72</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="9"/>
+        <v>7.8920909043478265</v>
+      </c>
+      <c r="D59" s="54">
+        <v>0.31800290000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="53">
+        <v>122.39</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="9"/>
+        <v>7.9221474608695654</v>
+      </c>
+      <c r="D60" s="54">
+        <v>3.0056556521739126E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="53">
+        <v>125</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="9"/>
+        <v>8.1459018260869573</v>
+      </c>
+      <c r="D61" s="54">
+        <v>0.22375436521739128</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="53">
+        <v>144.43</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="9"/>
+        <v>8.3464342521739141</v>
+      </c>
+      <c r="D62" s="54">
+        <v>0.20053242608695654</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="53">
+        <v>170.44</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="9"/>
+        <v>8.5040216608695669</v>
+      </c>
+      <c r="D63" s="54">
+        <v>0.15758740869565219</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="53">
+        <v>201.13</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="9"/>
+        <v>8.6222402608695674</v>
+      </c>
+      <c r="D64" s="54">
+        <v>0.11821860000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="53">
+        <v>237.35</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="9"/>
+        <v>8.649954221739133</v>
+      </c>
+      <c r="D65" s="54">
+        <v>2.7713960869565214E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="53">
+        <v>250</v>
+      </c>
+      <c r="C66" s="3">
+        <f>D66+C65</f>
+        <v>8.7158762130434813</v>
+      </c>
+      <c r="D66" s="54">
+        <v>6.5921991304347824E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="53">
+        <v>280.08999999999997</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" si="9"/>
+        <v>8.7468423260869592</v>
+      </c>
+      <c r="D67" s="54">
+        <v>3.0966113043478259E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="53">
+        <v>300</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="9"/>
+        <v>10.45890106956522</v>
+      </c>
+      <c r="D68" s="54">
+        <v>1.7120587434782608</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="53">
+        <v>330.52</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="9"/>
+        <v>13.774185308695655</v>
+      </c>
+      <c r="D69" s="54">
+        <v>3.3152842391304347</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="53">
+        <v>390.04</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="9"/>
+        <v>17.662748386956522</v>
+      </c>
+      <c r="D70" s="54">
+        <v>3.8885630782608689</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="53">
+        <v>460.27</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="9"/>
+        <v>38.970567352173916</v>
+      </c>
+      <c r="D71" s="54">
+        <v>21.30781896521739</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="53">
+        <v>850</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="9"/>
+        <v>47.13319511739131</v>
+      </c>
+      <c r="D72" s="54">
+        <v>8.1626277652173904</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="53">
+        <v>1000</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="9"/>
+        <v>100.00000011739129</v>
+      </c>
+      <c r="D73" s="54">
+        <v>52.866804999999992</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="60"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529AA10A-7A72-482C-95E8-4CA51D7B8E74}">
+  <dimension ref="B1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7426,720 +9477,778 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="79"/>
+      <c r="H2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="K2" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="15">
         <v>9</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="H2" s="18" t="s">
+      <c r="J3" s="14">
+        <f>I3/$I$9</f>
+        <v>0.21951219512195122</v>
+      </c>
+      <c r="K3" s="14">
+        <f>J3</f>
+        <v>0.21951219512195122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="12">
+        <v>9.359555488395413E-3</v>
+      </c>
+      <c r="D4" s="12">
+        <f>C4</f>
+        <v>9.359555488395413E-3</v>
+      </c>
+      <c r="E4" s="13">
+        <f>ROUNDUP(C4*1000,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="I4" s="15">
+        <v>2</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:J8" si="0">I4/$I$9</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="K4" s="14">
+        <f>J4+K3</f>
+        <v>0.26829268292682928</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>8.650709206137662E-3</v>
+      </c>
+      <c r="D5" s="12">
+        <f>C5+D4</f>
+        <v>1.8010264694533075E-2</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" ref="E5:E23" si="1">ROUNDUP(C5*1000,0)</f>
+        <v>9</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="0"/>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" ref="K5:K8" si="2">J5+K4</f>
+        <v>0.29268292682926833</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1.2320185113400368E-3</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" ref="D6:D23" si="3">C6+D5</f>
+        <v>1.9242283205873113E-2</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="15">
+        <v>26</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.63414634146341464</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="2"/>
+        <v>0.92682926829268297</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="12">
+        <v>6.6339458302924835E-4</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="3"/>
+        <v>1.990567778890236E-2</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="I7" s="15">
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="2"/>
+        <v>0.95121951219512202</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2.5343191042496417E-2</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="3"/>
+        <v>4.5248868831398781E-2</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2</v>
+      </c>
+      <c r="I8" s="11">
+        <v>2</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="C9" s="12">
+        <v>9.0497737556561458E-4</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="3"/>
+        <v>4.6153846206964395E-2</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="17">
+        <f>SUM(I3:I8)</f>
+        <v>41</v>
+      </c>
+      <c r="J9" s="17">
+        <f>SUM(J3:J8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <v>2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1.3574660633484115E-3</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="3"/>
+        <v>4.7511312270312807E-2</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="C11" s="23">
+        <v>1.8099547511312222E-3</v>
+      </c>
+      <c r="D11" s="23">
+        <f t="shared" si="3"/>
+        <v>4.9321267021444029E-2</v>
+      </c>
+      <c r="E11" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="22">
+        <v>4</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2.7149321266968368E-3</v>
+      </c>
+      <c r="D12" s="23">
+        <f t="shared" si="3"/>
+        <v>5.2036199148140866E-2</v>
+      </c>
+      <c r="E12" s="38">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="14">
+        <f>K5</f>
+        <v>0.29268292682926833</v>
+      </c>
+      <c r="I12" s="11">
+        <f>H5</f>
+        <v>0.7</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>5.6</v>
+      </c>
+      <c r="C13" s="23">
+        <v>3.6199095022624445E-3</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" si="3"/>
+        <v>5.565610865040331E-2</v>
+      </c>
+      <c r="E13" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="19">
+        <f>I12 + (H13 - H12) * ((I14 - I12) / (H14 - H12))</f>
+        <v>0.79807692307692302</v>
+      </c>
+      <c r="K13" s="21">
+        <f>I13</f>
+        <v>0.79807692307692302</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="22">
+        <v>8</v>
+      </c>
+      <c r="C14" s="23">
+        <v>5.4298642533936597E-3</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="3"/>
+        <v>6.108597290379697E-2</v>
+      </c>
+      <c r="E14" s="38">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H14" s="14">
+        <f>K6</f>
+        <v>0.92682926829268297</v>
+      </c>
+      <c r="I14" s="11">
+        <f>H6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="22">
+        <v>11</v>
+      </c>
+      <c r="C15" s="23">
+        <v>6.7873303167420851E-3</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="3"/>
+        <v>6.7873303220539055E-2</v>
+      </c>
+      <c r="E15" s="38">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="22">
         <v>16</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="18" t="s">
+      <c r="C16" s="23">
+        <v>4.5248868778280542E-2</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="3"/>
+        <v>0.1131221719988196</v>
+      </c>
+      <c r="E16" s="38">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H16" s="40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="22">
+        <v>22.6</v>
+      </c>
+      <c r="C17" s="23">
+        <v>0.11312217194570136</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.22624434394452098</v>
+      </c>
+      <c r="E17" s="38">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="17">
-        <v>9</v>
-      </c>
-      <c r="J3" s="16">
-        <f>I3/$I$8</f>
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="K3" s="16">
-        <f>J3</f>
-        <v>0.22500000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
-        <v>180</v>
-      </c>
-      <c r="C4" s="10">
-        <v>5.8823529411764719E-2</v>
-      </c>
-      <c r="D4" s="10">
-        <v>5.8823529411764719E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <f>ROUNDUP(C4*1000,0)</f>
-        <v>59</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="I4" s="17">
+      <c r="J17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="22">
+        <v>32</v>
+      </c>
+      <c r="C18" s="23">
+        <v>0.12217194570135746</v>
+      </c>
+      <c r="D18" s="23">
+        <f t="shared" si="3"/>
+        <v>0.34841628964587845</v>
+      </c>
+      <c r="E18" s="38">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="H18" s="22">
         <v>2</v>
       </c>
-      <c r="J4" s="16">
-        <f t="shared" ref="J4:J7" si="0">I4/$I$8</f>
-        <v>0.05</v>
-      </c>
-      <c r="K4" s="16">
-        <f>J4+K3</f>
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>128</v>
-      </c>
-      <c r="C5" s="10">
-        <v>4.5248868778280493E-2</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.10407239819004521</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" ref="E5:E22" si="1">ROUNDUP(C5*1000,0)</f>
-        <v>46</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1</v>
-      </c>
-      <c r="I5" s="17">
-        <v>26</v>
-      </c>
-      <c r="J5" s="16">
-        <f t="shared" si="0"/>
-        <v>0.65</v>
-      </c>
-      <c r="K5" s="16">
-        <f t="shared" ref="K5:K7" si="2">J5+K4</f>
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="I18" s="22">
+        <v>2</v>
+      </c>
+      <c r="J18" s="23">
+        <f>I18/$I$29</f>
+        <v>2.8694404591104736E-3</v>
+      </c>
+      <c r="K18" s="23">
+        <f>J18</f>
+        <v>2.8694404591104736E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="22">
+        <v>45</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0.19457013574660634</v>
+      </c>
+      <c r="D19" s="23">
+        <f t="shared" si="3"/>
+        <v>0.54298642539248476</v>
+      </c>
+      <c r="E19" s="38">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="H19" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="I19" s="25">
+        <v>2</v>
+      </c>
+      <c r="J19" s="23">
+        <f>I19/$I$29</f>
+        <v>2.8694404591104736E-3</v>
+      </c>
+      <c r="K19" s="23">
+        <f>J19+K18</f>
+        <v>5.7388809182209472E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="22">
+        <v>64</v>
+      </c>
+      <c r="C20" s="23">
+        <v>0.19457013574660634</v>
+      </c>
+      <c r="D20" s="23">
+        <f t="shared" si="3"/>
+        <v>0.73755656113909107</v>
+      </c>
+      <c r="E20" s="38">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="H20" s="22">
+        <v>4</v>
+      </c>
+      <c r="I20" s="25">
+        <v>3</v>
+      </c>
+      <c r="J20" s="23">
+        <f>I20/$I$29</f>
+        <v>4.30416068866571E-3</v>
+      </c>
+      <c r="K20" s="23">
+        <f t="shared" ref="K20:K28" si="4">J20+K19</f>
+        <v>1.0043041606886658E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="80">
         <v>90</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C21" s="81">
         <v>0.15837104072398189</v>
       </c>
-      <c r="D6" s="10">
-        <v>0.26244343891402711</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D21" s="81">
+        <f t="shared" si="3"/>
+        <v>0.89592760186307296</v>
+      </c>
+      <c r="E21" s="60">
         <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="H6" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="I6" s="17">
-        <v>1</v>
-      </c>
-      <c r="J6" s="16">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K6" s="16">
-        <f t="shared" si="2"/>
-        <v>0.95000000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="24">
-        <v>64</v>
-      </c>
-      <c r="C7" s="25">
-        <v>0.19457013574660631</v>
-      </c>
-      <c r="D7" s="25">
-        <v>0.45701357466063341</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>195</v>
-      </c>
-      <c r="H7" s="13">
-        <v>2</v>
-      </c>
-      <c r="I7" s="17">
-        <v>2</v>
-      </c>
-      <c r="J7" s="16">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-      <c r="K7" s="16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="24">
-        <v>45</v>
-      </c>
-      <c r="C8" s="25">
-        <v>0.19457013574660631</v>
-      </c>
-      <c r="D8" s="25">
-        <v>0.65158371040723972</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>195</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="19">
-        <f>SUM(I3:I7)</f>
-        <v>40</v>
-      </c>
-      <c r="J8" s="19">
-        <f t="shared" ref="J8" si="3">SUM(J3:J7)</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="19"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="24">
-        <v>32</v>
-      </c>
-      <c r="C9" s="25">
-        <v>0.12217194570135748</v>
-      </c>
-      <c r="D9" s="25">
-        <v>0.7737556561085972</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="24">
-        <v>22.6</v>
-      </c>
-      <c r="C10" s="25">
-        <v>0.11312217194570137</v>
-      </c>
-      <c r="D10" s="25">
-        <v>0.8868778280542986</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="24">
-        <v>16</v>
-      </c>
-      <c r="C11" s="25">
-        <v>4.5248868778280549E-2</v>
-      </c>
-      <c r="D11" s="25">
-        <v>0.9321266968325792</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="H21" s="22">
+        <v>5.6</v>
+      </c>
+      <c r="I21" s="25">
+        <v>4</v>
+      </c>
+      <c r="J21" s="23">
+        <f>I21/$I$29</f>
+        <v>5.7388809182209472E-3</v>
+      </c>
+      <c r="K21" s="23">
+        <f t="shared" si="4"/>
+        <v>1.5781922525107607E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>128</v>
+      </c>
+      <c r="C22" s="10">
+        <v>4.5248868778280542E-2</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="3"/>
+        <v>0.94117647064135346</v>
+      </c>
+      <c r="E22" s="1">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="H11" s="21">
-        <v>0.80153846153846098</v>
-      </c>
-      <c r="I11" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="23">
-        <f>H11</f>
-        <v>0.80153846153846098</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="24">
+      <c r="H22" s="22">
+        <v>8</v>
+      </c>
+      <c r="I22" s="25">
+        <v>6</v>
+      </c>
+      <c r="J22" s="23">
+        <f>I22/$I$29</f>
+        <v>8.60832137733142E-3</v>
+      </c>
+      <c r="K22" s="23">
+        <f t="shared" si="4"/>
+        <v>2.4390243902439025E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="57">
+        <v>180</v>
+      </c>
+      <c r="C23" s="81">
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0000000000531182</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="H23" s="22">
         <v>11</v>
       </c>
-      <c r="C12" s="25">
-        <v>6.7873303167420851E-3</v>
-      </c>
-      <c r="D12" s="25">
-        <v>0.93891402714932126</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="1"/>
+      <c r="I23" s="25">
         <v>7</v>
       </c>
-      <c r="H12" s="13">
+      <c r="J23" s="23">
+        <f>I23/$I$29</f>
+        <v>1.0043041606886656E-2</v>
+      </c>
+      <c r="K23" s="23">
+        <f t="shared" si="4"/>
+        <v>3.443328550932568E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <f>SUM(E4:E23)</f>
+        <v>1010</v>
+      </c>
+      <c r="H24" s="22">
+        <v>16</v>
+      </c>
+      <c r="I24" s="25">
+        <v>46</v>
+      </c>
+      <c r="J24" s="23">
+        <f>I24/$I$29</f>
+        <v>6.5997130559540887E-2</v>
+      </c>
+      <c r="K24" s="23">
+        <f t="shared" si="4"/>
+        <v>0.10043041606886657</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H25" s="22">
+        <v>22.6</v>
+      </c>
+      <c r="I25" s="25">
+        <v>114</v>
+      </c>
+      <c r="J25" s="23">
+        <f>I25/$I$29</f>
+        <v>0.16355810616929697</v>
+      </c>
+      <c r="K25" s="23">
+        <f t="shared" si="4"/>
+        <v>0.26398852223816355</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3">
+        <f>K32</f>
+        <v>34.766666666666666</v>
+      </c>
+      <c r="H26" s="22">
+        <v>32</v>
+      </c>
+      <c r="I26" s="25">
+        <v>123</v>
+      </c>
+      <c r="J26" s="23">
+        <f>I26/$I$29</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="K26" s="23">
+        <f t="shared" si="4"/>
+        <v>0.44045911047345765</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3">
+        <f>K13</f>
+        <v>0.79807692307692302</v>
+      </c>
+      <c r="H27" s="22">
+        <v>45</v>
+      </c>
+      <c r="I27" s="25">
+        <v>195</v>
+      </c>
+      <c r="J27" s="23">
+        <f>I27/$I$29</f>
+        <v>0.27977044476327118</v>
+      </c>
+      <c r="K27" s="23">
+        <f t="shared" si="4"/>
+        <v>0.72022955523672882</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="31">
+        <f>C26/C27</f>
+        <v>43.563052208835344</v>
+      </c>
+      <c r="H28" s="22">
+        <v>64</v>
+      </c>
+      <c r="I28" s="25">
+        <v>195</v>
+      </c>
+      <c r="J28" s="23">
+        <f>I28/$I$29</f>
+        <v>0.27977044476327118</v>
+      </c>
+      <c r="K28" s="23">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="I12" s="16">
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="24">
-        <v>8</v>
-      </c>
-      <c r="C13" s="25">
-        <v>5.4298642533936597E-3</v>
-      </c>
-      <c r="D13" s="25">
-        <v>0.94434389140271491</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="24">
-        <v>5.6</v>
-      </c>
-      <c r="C14" s="25">
-        <v>3.6199095022624445E-3</v>
-      </c>
-      <c r="D14" s="25">
-        <v>0.94796380090497734</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H14" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="24">
-        <v>4</v>
-      </c>
-      <c r="C15" s="25">
-        <v>2.7149321266968368E-3</v>
-      </c>
-      <c r="D15" s="25">
-        <v>0.95067873303167416</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="18" t="s">
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="24">
-        <v>2.8</v>
-      </c>
-      <c r="C16" s="25">
-        <v>1.8099547511312222E-3</v>
-      </c>
-      <c r="D16" s="25">
-        <v>0.95248868778280538</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H16" s="24">
-        <v>2</v>
-      </c>
-      <c r="I16" s="24">
-        <v>2</v>
-      </c>
-      <c r="J16" s="25">
-        <f>I16/$I$27</f>
-        <v>2.8694404591104736E-3</v>
-      </c>
-      <c r="K16" s="25">
-        <f>J16</f>
-        <v>2.8694404591104736E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="13">
-        <v>2</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1.3574660633484115E-3</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0.95384615384615379</v>
-      </c>
-      <c r="E17" s="15">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H17" s="24">
-        <v>2.8</v>
-      </c>
-      <c r="I17" s="27">
-        <v>2</v>
-      </c>
-      <c r="J17" s="25">
-        <f t="shared" ref="J17:J26" si="4">I17/$I$27</f>
-        <v>2.8694404591104736E-3</v>
-      </c>
-      <c r="K17" s="25">
-        <f>J17+K16</f>
-        <v>5.7388809182209472E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="C18" s="14">
-        <v>9.0497737556561458E-4</v>
-      </c>
-      <c r="D18" s="14">
-        <v>0.9547511312217194</v>
-      </c>
-      <c r="E18" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H18" s="24">
-        <v>4</v>
-      </c>
-      <c r="I18" s="27">
-        <v>3</v>
-      </c>
-      <c r="J18" s="25">
-        <f t="shared" si="4"/>
-        <v>4.30416068866571E-3</v>
-      </c>
-      <c r="K18" s="25">
-        <f t="shared" ref="K18:K26" si="5">J18+K17</f>
-        <v>1.0043041606886658E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="13">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14">
-        <v>2.5343191042496417E-2</v>
-      </c>
-      <c r="D19" s="14">
-        <v>0.98009432226421578</v>
-      </c>
-      <c r="E19" s="15">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="H19" s="24">
-        <v>5.6</v>
-      </c>
-      <c r="I19" s="27">
-        <v>4</v>
-      </c>
-      <c r="J19" s="25">
-        <f t="shared" si="4"/>
-        <v>5.7388809182209472E-3</v>
-      </c>
-      <c r="K19" s="25">
-        <f t="shared" si="5"/>
-        <v>1.5781922525107607E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="C20" s="14">
-        <v>1.8954130943692853E-3</v>
-      </c>
-      <c r="D20" s="14">
-        <v>0.98198973535858503</v>
-      </c>
-      <c r="E20" s="15">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H20" s="24">
-        <v>8</v>
-      </c>
-      <c r="I20" s="27">
-        <v>6</v>
-      </c>
-      <c r="J20" s="25">
-        <f t="shared" si="4"/>
-        <v>8.60832137733142E-3</v>
-      </c>
-      <c r="K20" s="25">
-        <f t="shared" si="5"/>
-        <v>2.4390243902439025E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="C21" s="14">
-        <v>8.650709206137662E-3</v>
-      </c>
-      <c r="D21" s="14">
-        <v>0.99064044456472267</v>
-      </c>
-      <c r="E21" s="15">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="H21" s="24">
-        <v>11</v>
-      </c>
-      <c r="I21" s="27">
-        <v>7</v>
-      </c>
-      <c r="J21" s="25">
-        <f t="shared" si="4"/>
-        <v>1.0043041606886656E-2</v>
-      </c>
-      <c r="K21" s="25">
-        <f t="shared" si="5"/>
-        <v>3.443328550932568E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="10">
-        <v>9.3595554883954112E-3</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1.0000000000531182</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="H22" s="24">
-        <v>16</v>
-      </c>
-      <c r="I22" s="27">
-        <v>46</v>
-      </c>
-      <c r="J22" s="25">
-        <f t="shared" si="4"/>
-        <v>6.5997130559540887E-2</v>
-      </c>
-      <c r="K22" s="25">
-        <f t="shared" si="5"/>
-        <v>0.10043041606886657</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="I29" s="17">
+        <f>SUM(I18:I28)</f>
+        <v>697</v>
+      </c>
+      <c r="J29" s="17">
+        <f t="shared" ref="J29" si="5">SUM(J24:J28)</f>
+        <v>0.96556671449067433</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C23" s="32">
-        <v>59.8102564102564</v>
-      </c>
-      <c r="E23" s="1">
-        <f>SUM(E4:E22)</f>
-        <v>1009</v>
-      </c>
-      <c r="H23" s="24">
-        <v>22.6</v>
-      </c>
-      <c r="I23" s="27">
-        <v>114</v>
-      </c>
-      <c r="J23" s="25">
-        <f t="shared" si="4"/>
-        <v>0.16355810616929697</v>
-      </c>
-      <c r="K23" s="25">
-        <f t="shared" si="5"/>
-        <v>0.26398852223816355</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="24">
-        <v>32</v>
-      </c>
-      <c r="I24" s="27">
-        <v>123</v>
-      </c>
-      <c r="J24" s="25">
-        <f t="shared" si="4"/>
-        <v>0.17647058823529413</v>
-      </c>
-      <c r="K24" s="25">
-        <f t="shared" si="5"/>
-        <v>0.44045911047345765</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H25" s="24">
-        <v>45</v>
-      </c>
-      <c r="I25" s="27">
-        <v>195</v>
-      </c>
-      <c r="J25" s="25">
-        <f t="shared" si="4"/>
-        <v>0.27977044476327118</v>
-      </c>
-      <c r="K25" s="25">
-        <f t="shared" si="5"/>
-        <v>0.72022955523672882</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H26" s="24">
-        <v>64</v>
-      </c>
-      <c r="I26" s="27">
-        <v>195</v>
-      </c>
-      <c r="J26" s="25">
-        <f t="shared" si="4"/>
-        <v>0.27977044476327118</v>
-      </c>
-      <c r="K26" s="25">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="3">
-        <f>K30</f>
-        <v>34.785714285714199</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="19">
-        <f>SUM(I16:I26)</f>
-        <v>697</v>
-      </c>
-      <c r="J27" s="19">
-        <f t="shared" ref="J27" si="6">SUM(J22:J26)</f>
-        <v>0.96556671449067433</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="3">
-        <f>K11</f>
-        <v>0.80153846153846098</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E29" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="34">
-        <f>F27/F28</f>
-        <v>43.398683849739434</v>
-      </c>
-      <c r="H29" s="24">
-        <f>H24</f>
-        <v>32</v>
-      </c>
-      <c r="I29" s="26">
-        <f>K24</f>
-        <v>0.44045911047345765</v>
-      </c>
-      <c r="K29" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H30" s="29">
-        <v>34.785714285714199</v>
-      </c>
-      <c r="I30" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K30" s="31">
-        <f>H30</f>
-        <v>34.785714285714199</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H31" s="24">
-        <f>H25</f>
+        <f>K26</f>
+        <v>0.44045911047345765</v>
+      </c>
+      <c r="I31" s="22">
+        <f>H26</f>
+        <v>32</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G32" s="3"/>
+      <c r="H32" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="I32" s="27">
+        <f>I31 + (H32 - H31) * ((I33 - I31) / (H33 - H31))</f>
+        <v>34.766666666666666</v>
+      </c>
+      <c r="K32" s="29">
+        <f>I32</f>
+        <v>34.766666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="24">
+        <f>K27</f>
+        <v>0.72022955523672882</v>
+      </c>
+      <c r="I33" s="22">
+        <f>H27</f>
         <v>45</v>
       </c>
-      <c r="I31" s="26">
-        <f>K25</f>
-        <v>0.72022955523672882</v>
-      </c>
-    </row>
-    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H35" s="1"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADFD080-C3B6-452C-9963-E899A3982E0E}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
@@ -8158,28 +10267,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="48"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8208,11 +10317,11 @@
         <f>$I$20+($I$19-$I$20)*EXP(-14*A2)</f>
         <v>1.3290468742698638</v>
       </c>
-      <c r="H2" s="48" t="str">
+      <c r="H2" s="41" t="str">
         <f>B1</f>
         <v>Tri* (Dg/Ds = 10)</v>
       </c>
-      <c r="I2" s="48"/>
+      <c r="I2" s="41"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8340,11 +10449,11 @@
         <f t="shared" si="4"/>
         <v>0.7870350317127095</v>
       </c>
-      <c r="H6" s="48" t="str">
+      <c r="H6" s="41" t="str">
         <f>C1</f>
         <v>Tri* (Dg/Ds = 20)</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -8472,11 +10581,11 @@
         <f t="shared" si="4"/>
         <v>0.4774329545306662</v>
       </c>
-      <c r="H10" s="48" t="str">
+      <c r="H10" s="41" t="str">
         <f>D1</f>
         <v>Tri* (Dg/Ds = 35)</v>
       </c>
-      <c r="I10" s="48"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -8604,11 +10713,11 @@
         <f t="shared" si="4"/>
         <v>0.30058544185786273</v>
       </c>
-      <c r="H14" s="48" t="str">
+      <c r="H14" s="41" t="str">
         <f>E1</f>
         <v>Tri* (Dg/Ds = 50)</v>
       </c>
-      <c r="I14" s="48"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -8733,11 +10842,11 @@
         <f t="shared" si="4"/>
         <v>0.1995685397000391</v>
       </c>
-      <c r="H18" s="48" t="str">
+      <c r="H18" s="41" t="str">
         <f>F1</f>
         <v>Tri* (Dg/Ds = 43.4)</v>
       </c>
-      <c r="I18" s="48"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -9164,7 +11273,7 @@
         <v>7</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -9256,7 +11365,7 @@
       <c r="M35" s="6">
         <v>0.96462000000000003</v>
       </c>
-      <c r="N35" s="35">
+      <c r="N35" s="32">
         <v>0.86746324999999902</v>
       </c>
     </row>
@@ -11013,12 +13122,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE20B856-AC4B-4A0B-8068-FF571A1CD20B}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11041,26 +13150,26 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="8">
         <v>0.5</v>
@@ -11080,9 +13189,9 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="36">
+        <v>27</v>
+      </c>
+      <c r="B3" s="33">
         <v>0.21715999999999999</v>
       </c>
       <c r="C3" s="10">
@@ -11108,9 +13217,9 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="39">
+        <v>28</v>
+      </c>
+      <c r="B4" s="36">
         <v>0.40402499999999902</v>
       </c>
       <c r="C4" s="10">
@@ -11136,9 +13245,9 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="39">
+        <v>29</v>
+      </c>
+      <c r="B5" s="36">
         <v>0.68432000000000004</v>
       </c>
       <c r="C5" s="10">
@@ -11164,9 +13273,9 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="36">
+        <v>30</v>
+      </c>
+      <c r="B6" s="33">
         <v>0.96462000000000003</v>
       </c>
       <c r="C6" s="10">
@@ -11192,28 +13301,28 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="37">
+        <v>31</v>
+      </c>
+      <c r="B7" s="34">
         <v>0.86746324999999902</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <f>$B7*($B$11-$B$10)*$B$12*(C$2/1000)</f>
         <v>7.0181994965053045</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <f>$B7*($B$11-$B$10)*$B$12*(D$2/1000)</f>
         <v>10.527299244757957</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <f>$B7*($B$11-$B$10)*$B$12*(E$2/1000)</f>
         <v>14.036398993010609</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <f>$B7*($B$11-$B$10)*$B$12*(F$2/1000)</f>
         <v>21.054598489515914</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <f>$B7*($B$11-$B$10)*$B$12*(G$2/1000)</f>
         <v>28.072797986021218</v>
       </c>
@@ -11234,46 +13343,46 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="19">
+        <v>34</v>
+      </c>
+      <c r="B10" s="17">
         <v>1000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="19">
+        <v>36</v>
+      </c>
+      <c r="B11" s="17">
         <v>2650</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2">
         <v>9.8066499999999994</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12">
         <v>10.16</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="35">
         <f>F12/((B11-B10)*B12*(59/1000))</f>
         <v>1.0642338699389575E-2</v>
       </c>
@@ -11298,21 +13407,21 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
-        <v>43</v>
+      <c r="A16" s="37" t="s">
+        <v>41</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -11320,15 +13429,15 @@
       <c r="E16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
-        <v>33</v>
+      <c r="B17" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="42">
+      <c r="A18" s="8">
         <v>2</v>
       </c>
       <c r="B18" s="2">
@@ -11340,7 +13449,7 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="42">
+      <c r="A19" s="8">
         <v>20</v>
       </c>
       <c r="B19" s="2">
@@ -11352,7 +13461,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="42">
+      <c r="A20" s="8">
         <v>45</v>
       </c>
       <c r="B20" s="2">
@@ -11364,7 +13473,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="42">
+      <c r="A21" s="8">
         <v>63</v>
       </c>
       <c r="B21" s="2">
@@ -11376,7 +13485,7 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+      <c r="A22" s="8">
         <v>100</v>
       </c>
       <c r="B22" s="2">
@@ -11388,7 +13497,7 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="43">
+      <c r="A23" s="8">
         <v>200</v>
       </c>
       <c r="B23" s="2">
@@ -11400,7 +13509,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
+      <c r="A24" s="8">
         <v>280</v>
       </c>
       <c r="B24" s="2">
@@ -11412,7 +13521,7 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="43">
+      <c r="A25" s="8">
         <v>500</v>
       </c>
       <c r="B25" s="2">
@@ -11424,7 +13533,7 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
+      <c r="A26" s="8">
         <v>700</v>
       </c>
       <c r="B26" s="2">
@@ -11436,7 +13545,7 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="43">
+      <c r="A27" s="8">
         <v>850</v>
       </c>
       <c r="B27" s="2">
@@ -11448,7 +13557,7 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="8">
         <v>1000</v>
       </c>
       <c r="B28" s="2">
@@ -11460,7 +13569,7 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="40">
+      <c r="A29" s="8">
         <v>1500</v>
       </c>
       <c r="B29" s="2">
@@ -11472,7 +13581,7 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="43">
+      <c r="A30" s="8">
         <v>2000</v>
       </c>
       <c r="B30" s="2">

</xml_diff>

<commit_message>
updated a cell in wilcock 2002 calculations
</commit_message>
<xml_diff>
--- a/data/bedload_tauc/Wilcock2002_tauc.xlsx
+++ b/data/bedload_tauc/Wilcock2002_tauc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\sediment_trap_paper\data\bedload_tauc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data\bedload_tauc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C620D067-0743-4346-AC34-48F3412F6E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6AD99E-FAF4-4A5C-A2C4-04C2A7A98145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
   </bookViews>
   <sheets>
     <sheet name="Sand GSD calculations" sheetId="4" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Fs</t>
   </si>
@@ -280,6 +280,9 @@
   <si>
     <t xml:space="preserve">FINAL GSD - including sand sizes! </t>
   </si>
+  <si>
+    <t>Fines (&lt;0.5)</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +294,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,12 +331,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -510,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -622,27 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -651,9 +627,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -668,28 +641,13 @@
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,29 +665,33 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -739,13 +701,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7707,32 +7672,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="71" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="70"/>
+      <c r="G2" s="63"/>
       <c r="J2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7766,9 +7731,8 @@
         <f>K3</f>
         <v>9.359555488395413E-3</v>
       </c>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="73"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -7777,18 +7741,18 @@
       <c r="C4" s="9">
         <v>10</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="39">
         <v>0</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="40">
         <f>D4/$D$18*100</f>
         <v>0</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="56">
         <f>SUM(L32:L42)</f>
         <v>1.990567778890236E-2</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="55">
         <f>F4</f>
         <v>1.990567778890236E-2</v>
       </c>
@@ -7803,22 +7767,21 @@
         <f>K4+L3</f>
         <v>1.8010264694533075E-2</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="73"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="55">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="2">
         <f>L43</f>
         <v>2.5343191042496417E-2</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="2">
         <f>F5+G4</f>
         <v>4.5248868831398781E-2</v>
       </c>
@@ -7830,16 +7793,13 @@
         <v>1.2320185113400368E-3</v>
       </c>
       <c r="L5" s="10">
-        <f t="shared" ref="L5:L22" si="1">K5+L4</f>
+        <f t="shared" ref="L5:L6" si="1">K5+L4</f>
         <v>1.9242283205873113E-2</v>
       </c>
-      <c r="M5" s="74"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
@@ -7852,16 +7812,16 @@
         <f>C6+D4</f>
         <v>0</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="42">
         <f>D6/$D$18*100</f>
         <v>0</v>
       </c>
-      <c r="F6" s="69">
+      <c r="F6" s="3">
         <f>C6/$C$19</f>
         <v>0</v>
       </c>
-      <c r="G6" s="55">
-        <f t="shared" ref="G6:G18" si="2">F6+G5</f>
+      <c r="G6" s="2">
+        <f t="shared" ref="G6:G17" si="2">F6+G5</f>
         <v>4.5248868831398781E-2</v>
       </c>
       <c r="J6" s="11">
@@ -7875,13 +7835,12 @@
         <f t="shared" si="1"/>
         <v>1.990567778890236E-2</v>
       </c>
-      <c r="M6" s="74"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
@@ -7894,15 +7853,15 @@
         <f t="shared" ref="D7:D17" si="3">C7+D6</f>
         <v>0</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="42">
         <f t="shared" ref="E7:E17" si="4">D7/$D$18*100</f>
         <v>0</v>
       </c>
-      <c r="F7" s="69">
-        <f t="shared" ref="F7:F18" si="5">C7/$C$19</f>
+      <c r="F7" s="3">
+        <f t="shared" ref="F7:F17" si="5">C7/$C$19</f>
         <v>0</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
         <v>4.5248868831398781E-2</v>
       </c>
@@ -7917,13 +7876,12 @@
         <f>K7+L6</f>
         <v>4.5248868831398781E-2</v>
       </c>
-      <c r="M7" s="74"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="50"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
@@ -7936,15 +7894,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="42">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F8" s="69">
+      <c r="F8" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="2">
         <f t="shared" si="2"/>
         <v>4.5248868831398781E-2</v>
       </c>
@@ -7959,13 +7917,12 @@
         <f>$G$21*J8+$G$22</f>
         <v>4.6153846206964395E-2</v>
       </c>
-      <c r="M8" s="74"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="50"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
@@ -7978,15 +7935,15 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="42">
         <f t="shared" si="4"/>
         <v>2.3696682464454977</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F9" s="3">
         <f t="shared" si="5"/>
         <v>2.2624434389140271E-2</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="2">
         <f t="shared" si="2"/>
         <v>6.7873303220539055E-2</v>
       </c>
@@ -8001,13 +7958,12 @@
         <f>$G$21*J9+$G$22</f>
         <v>4.7511312270312807E-2</v>
       </c>
-      <c r="M9" s="74"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="50"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="1"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
@@ -8020,15 +7976,15 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="42">
         <f t="shared" si="4"/>
         <v>7.109004739336493</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F10" s="3">
         <f t="shared" si="5"/>
         <v>4.5248868778280542E-2</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="2">
         <f t="shared" si="2"/>
         <v>0.1131221719988196</v>
       </c>
@@ -8043,13 +7999,12 @@
         <f>$G$21*J10+$G$22</f>
         <v>4.9321267021444029E-2</v>
       </c>
-      <c r="M10" s="74"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="50"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="1"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
@@ -8062,15 +8017,15 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="42">
         <f t="shared" si="4"/>
         <v>18.957345971563981</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F11" s="3">
         <f t="shared" si="5"/>
         <v>0.11312217194570136</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="2">
         <f t="shared" si="2"/>
         <v>0.22624434394452098</v>
       </c>
@@ -8085,34 +8040,33 @@
         <f>$G$21*J11+$G$22</f>
         <v>5.2036199148140866E-2</v>
       </c>
-      <c r="M11" s="74"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="50"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="51">
+      <c r="B12" s="43">
         <v>32</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="43">
         <v>27</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="43">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="44">
         <f t="shared" si="4"/>
         <v>31.753554502369667</v>
       </c>
-      <c r="F12" s="69">
+      <c r="F12" s="3">
         <f t="shared" si="5"/>
         <v>0.12217194570135746</v>
       </c>
-      <c r="G12" s="55">
+      <c r="G12" s="2">
         <f t="shared" si="2"/>
         <v>0.34841628964587845</v>
       </c>
@@ -8127,34 +8081,33 @@
         <f t="shared" ref="L12:L13" si="7">$G$21*J12+$G$22</f>
         <v>5.565610865040331E-2</v>
       </c>
-      <c r="M12" s="74"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="50"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="1"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="51">
+      <c r="B13" s="43">
         <v>45</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="43">
         <v>43</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="43">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="44">
         <f t="shared" si="4"/>
         <v>52.132701421800952</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F13" s="3">
         <f t="shared" si="5"/>
         <v>0.19457013574660634</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="2">
         <f t="shared" si="2"/>
         <v>0.54298642539248476</v>
       </c>
@@ -8169,13 +8122,12 @@
         <f t="shared" si="7"/>
         <v>6.108597290379697E-2</v>
       </c>
-      <c r="M13" s="74"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="73"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="50"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="1"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
@@ -8188,15 +8140,15 @@
         <f t="shared" si="3"/>
         <v>153</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E14" s="42">
         <f t="shared" si="4"/>
         <v>72.511848341232238</v>
       </c>
-      <c r="F14" s="69">
+      <c r="F14" s="3">
         <f t="shared" si="5"/>
         <v>0.19457013574660634</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
         <v>0.73755656113909107</v>
       </c>
@@ -8211,13 +8163,12 @@
         <f>G9</f>
         <v>6.7873303220539055E-2</v>
       </c>
-      <c r="M14" s="74"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="50"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
@@ -8230,15 +8181,15 @@
         <f t="shared" si="3"/>
         <v>188</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="42">
         <f t="shared" si="4"/>
         <v>89.099526066350705</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="3">
         <f t="shared" si="5"/>
         <v>0.15837104072398189</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15" s="2">
         <f t="shared" si="2"/>
         <v>0.89592760186307296</v>
       </c>
@@ -8246,20 +8197,19 @@
         <v>16</v>
       </c>
       <c r="K15" s="23">
-        <f>F10</f>
+        <f t="shared" ref="K15:K22" si="8">F10</f>
         <v>4.5248868778280542E-2</v>
       </c>
       <c r="L15" s="10">
         <f>K15+L14</f>
         <v>0.1131221719988196</v>
       </c>
-      <c r="M15" s="74"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="50"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="1"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
@@ -8272,15 +8222,15 @@
         <f t="shared" si="3"/>
         <v>198</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E16" s="42">
         <f t="shared" si="4"/>
         <v>93.838862559241704</v>
       </c>
-      <c r="F16" s="69">
+      <c r="F16" s="3">
         <f t="shared" si="5"/>
         <v>4.5248868778280542E-2</v>
       </c>
-      <c r="G16" s="55">
+      <c r="G16" s="2">
         <f t="shared" si="2"/>
         <v>0.94117647064135346</v>
       </c>
@@ -8288,20 +8238,19 @@
         <v>22.6</v>
       </c>
       <c r="K16" s="23">
-        <f>F11</f>
+        <f t="shared" si="8"/>
         <v>0.11312217194570136</v>
       </c>
       <c r="L16" s="10">
-        <f t="shared" ref="L16:L22" si="8">K16+L15</f>
+        <f t="shared" ref="L16:L22" si="9">K16+L15</f>
         <v>0.22624434394452098</v>
       </c>
-      <c r="M16" s="74"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="50"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="1"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
@@ -8314,15 +8263,15 @@
         <f t="shared" si="3"/>
         <v>211</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="42">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="F17" s="69">
+      <c r="F17" s="3">
         <f t="shared" si="5"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G17" s="55">
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
         <v>1.0000000000531182</v>
       </c>
@@ -8330,20 +8279,19 @@
         <v>32</v>
       </c>
       <c r="K17" s="23">
-        <f>F12</f>
+        <f t="shared" si="8"/>
         <v>0.12217194570135746</v>
       </c>
       <c r="L17" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.34841628964587845</v>
       </c>
-      <c r="M17" s="74"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="50"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="1"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
@@ -8356,29 +8304,28 @@
         <v>211</v>
       </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="69">
+      <c r="F18" s="3">
         <f>SUM(F4:F17)</f>
         <v>1.0000000000531182</v>
       </c>
-      <c r="G18" s="55"/>
+      <c r="G18" s="2"/>
       <c r="J18" s="22">
         <v>45</v>
       </c>
       <c r="K18" s="23">
-        <f>F13</f>
+        <f t="shared" si="8"/>
         <v>0.19457013574660634</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.54298642539248476</v>
       </c>
-      <c r="M18" s="74"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="S18" s="50"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="1"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -8396,30 +8343,29 @@
         <v>64</v>
       </c>
       <c r="K19" s="23">
-        <f>F14</f>
+        <f t="shared" si="8"/>
         <v>0.19457013574660634</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.73755656113909107</v>
       </c>
-      <c r="M19" s="74"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74"/>
-      <c r="S19" s="50"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="1"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="52">
         <f>C4/C19*100</f>
         <v>4.5248868778280542</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="47" t="s">
         <v>69</v>
       </c>
       <c r="G20" s="1"/>
@@ -8427,26 +8373,25 @@
         <v>90</v>
       </c>
       <c r="K20" s="10">
-        <f>F15</f>
+        <f t="shared" si="8"/>
         <v>0.15837104072398189</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.89592760186307296</v>
       </c>
-      <c r="M20" s="74"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="50"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="1"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="67">
+      <c r="G21" s="54">
         <f>(G5-G9)/(B5-B9)</f>
         <v>2.2624434389140274E-3</v>
       </c>
@@ -8454,23 +8399,22 @@
         <v>128</v>
       </c>
       <c r="K21" s="10">
-        <f>F16</f>
+        <f t="shared" si="8"/>
         <v>4.5248868778280542E-2</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.94117647064135346</v>
       </c>
-      <c r="M21" s="74"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="50"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="1"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -8484,20 +8428,19 @@
         <v>180</v>
       </c>
       <c r="K22" s="10">
-        <f>F17</f>
+        <f t="shared" si="8"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0000000000531182</v>
       </c>
-      <c r="M22" s="74"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="73"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="50"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="1"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
@@ -8513,112 +8456,103 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="N23" s="1"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74"/>
-      <c r="S23" s="50"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="1"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="53">
+      <c r="B24" s="45">
         <v>0.37</v>
       </c>
       <c r="C24" s="3">
         <f>D24</f>
         <v>1.4521943478260869E-2</v>
       </c>
-      <c r="D24" s="54">
+      <c r="D24" s="46">
         <v>1.4521943478260869E-2</v>
       </c>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="74"/>
-      <c r="R24" s="74"/>
-      <c r="S24" s="50"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="1"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="53">
+      <c r="B25" s="45">
         <v>0.44</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" ref="C25:C73" si="9">D25+C24</f>
+        <f t="shared" ref="C25:C73" si="10">D25+C24</f>
         <v>2.9906226086956519E-2</v>
       </c>
-      <c r="D25" s="54">
+      <c r="D25" s="46">
         <v>1.5384282608695652E-2</v>
       </c>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="50"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="1"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="53">
+      <c r="B26" s="45">
         <v>0.52</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.6655078260869565E-2</v>
       </c>
-      <c r="D26" s="54">
+      <c r="D26" s="46">
         <v>1.6748852173913042E-2</v>
       </c>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="50"/>
-      <c r="R26" s="76"/>
-      <c r="S26" s="50"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="1"/>
+      <c r="S26" s="1"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="53">
+      <c r="B27" s="45">
         <v>0.61</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.5399752173913042E-2</v>
       </c>
-      <c r="D27" s="54">
+      <c r="D27" s="46">
         <v>1.8744673913043474E-2</v>
       </c>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
-      <c r="S27" s="76"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="53">
+      <c r="B28" s="45">
         <v>0.72</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.6922495652173914E-2</v>
       </c>
-      <c r="D28" s="54">
+      <c r="D28" s="46">
         <v>2.1522743478260869E-2</v>
       </c>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="76"/>
-      <c r="S28" s="76"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="53">
+      <c r="B29" s="45">
         <v>0.85</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.11223754782608694</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D29" s="46">
         <v>2.5315052173913034E-2</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="53">
+      <c r="B30" s="45">
         <v>1.01</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.14369522173913041</v>
       </c>
-      <c r="D30" s="54">
+      <c r="D30" s="46">
         <v>3.1457673913043473E-2</v>
       </c>
       <c r="G30" t="s">
@@ -8629,20 +8563,20 @@
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="53">
+      <c r="B31" s="45">
         <v>1.19</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.18734088260869564</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D31" s="46">
         <v>4.3645660869565228E-2</v>
       </c>
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="63" t="s">
+      <c r="G31" s="50" t="s">
         <v>56</v>
       </c>
       <c r="H31" s="8" t="s">
@@ -8651,7 +8585,7 @@
       <c r="I31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K31" s="63" t="s">
+      <c r="K31" s="50" t="s">
         <v>56</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -8659,24 +8593,24 @@
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="53">
+      <c r="B32" s="45">
         <v>1.4</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.25067402608695649</v>
       </c>
-      <c r="D32" s="54">
+      <c r="D32" s="46">
         <v>6.333314347826087E-2</v>
       </c>
-      <c r="F32" s="59">
+      <c r="F32" s="48">
         <v>1</v>
       </c>
-      <c r="G32" s="63">
+      <c r="G32" s="50">
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="H32" s="49">
+      <c r="H32" s="42">
         <f>C30</f>
         <v>0.14369522173913041</v>
       </c>
@@ -8684,34 +8618,34 @@
         <f>H32</f>
         <v>0.14369522173913041</v>
       </c>
-      <c r="K32" s="63">
+      <c r="K32" s="50">
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="L32" s="66">
+      <c r="L32" s="53">
         <f>I32*$C$20/10000</f>
         <v>6.5020462325398381E-5</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="53">
+      <c r="B33" s="45">
         <v>1.65</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.329392652173913</v>
       </c>
-      <c r="D33" s="54">
+      <c r="D33" s="46">
         <v>7.8718626086956511E-2</v>
       </c>
-      <c r="F33" s="59">
+      <c r="F33" s="48">
         <v>5</v>
       </c>
-      <c r="G33" s="63">
+      <c r="G33" s="50">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H33" s="49">
+      <c r="H33" s="42">
         <f>C39 + (F33 - B39) * ((C40 - C39) / (B40 - B39))</f>
         <v>1.1092679565217392</v>
       </c>
@@ -8719,241 +8653,241 @@
         <f>H33-H32</f>
         <v>0.96557273478260874</v>
       </c>
-      <c r="K33" s="63">
+      <c r="K33" s="50">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L33" s="66">
-        <f t="shared" ref="L33:L43" si="10">I33*$C$20/10000</f>
+      <c r="L33" s="53">
+        <f t="shared" ref="L33:L43" si="11">I33*$C$20/10000</f>
         <v>4.3691073972063743E-4</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="53">
+      <c r="B34" s="45">
         <v>1.95</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.42033431739130428</v>
       </c>
-      <c r="D34" s="54">
+      <c r="D34" s="46">
         <v>9.094166521739129E-2</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F34" s="48">
         <v>10</v>
       </c>
-      <c r="G34" s="63">
+      <c r="G34" s="50">
         <f>10/1000</f>
         <v>0.01</v>
       </c>
-      <c r="H34" s="49">
+      <c r="H34" s="42">
         <f>C43 + (F34 - B43) * ((C44 - C43) / (B44 - B43))</f>
         <v>1.8372186405518396</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" ref="I34:I42" si="11">H34-H33</f>
+        <f t="shared" ref="I34:I39" si="12">H34-H33</f>
         <v>0.72795068403010044</v>
       </c>
-      <c r="K34" s="63">
+      <c r="K34" s="50">
         <f>10/1000</f>
         <v>0.01</v>
       </c>
-      <c r="L34" s="66">
+      <c r="L34" s="53">
+        <f t="shared" si="11"/>
+        <v>3.2938944978737577E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="45">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C35" s="3">
         <f t="shared" si="10"/>
-        <v>3.2938944978737577E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="53">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="9"/>
         <v>0.52298628260869562</v>
       </c>
-      <c r="D35" s="54">
+      <c r="D35" s="46">
         <v>0.10265196521739132</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="48">
         <v>50</v>
       </c>
-      <c r="G35" s="63">
+      <c r="G35" s="50">
         <f>50/1000</f>
         <v>0.05</v>
       </c>
-      <c r="H35" s="49">
+      <c r="H35" s="42">
         <f>C54 + (F35 - B54) * ((C55 - C54) / (B55 - B54))</f>
         <v>5.8736056187979546</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.0363869782461155</v>
       </c>
-      <c r="K35" s="63">
+      <c r="K35" s="50">
         <f>50/1000</f>
         <v>0.05</v>
       </c>
-      <c r="L35" s="66">
+      <c r="L35" s="53">
+        <f t="shared" si="11"/>
+        <v>1.8264194471701882E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="45">
+        <v>2.72</v>
+      </c>
+      <c r="C36" s="3">
         <f t="shared" si="10"/>
-        <v>1.8264194471701882E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="53">
-        <v>2.72</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="9"/>
         <v>0.63402316086956523</v>
       </c>
-      <c r="D36" s="54">
+      <c r="D36" s="46">
         <v>0.11103687826086958</v>
       </c>
-      <c r="F36" s="59">
+      <c r="F36" s="48">
         <v>100</v>
       </c>
-      <c r="G36" s="63">
+      <c r="G36" s="50">
         <f>100/1000</f>
         <v>0.1</v>
       </c>
-      <c r="H36" s="49">
+      <c r="H36" s="42">
         <f>C58 + (F36 - B58) * ((C59 - C58) / (B59 - B58))</f>
         <v>7.8173612272789699</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.9437556084810153</v>
       </c>
-      <c r="K36" s="63">
+      <c r="K36" s="50">
         <f>100/1000</f>
         <v>0.1</v>
       </c>
-      <c r="L36" s="66">
+      <c r="L36" s="53">
+        <f t="shared" si="11"/>
+        <v>8.7952742465204319E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="C37" s="3">
         <f t="shared" si="10"/>
-        <v>8.7952742465204319E-4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="53">
-        <v>3.2</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="9"/>
         <v>0.75186232608695658</v>
       </c>
-      <c r="D37" s="54">
+      <c r="D37" s="46">
         <v>0.11783916521739132</v>
       </c>
-      <c r="F37" s="59">
+      <c r="F37" s="48">
         <v>200</v>
       </c>
-      <c r="G37" s="63">
+      <c r="G37" s="50">
         <f>200/1000</f>
         <v>0.2</v>
       </c>
-      <c r="H37" s="49">
+      <c r="H37" s="42">
         <f>C63 + (F37 - B63) * ((C64 - C63) / (B64 - B63))</f>
         <v>8.6178874743593035</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.8005262470803336</v>
       </c>
-      <c r="K37" s="63">
+      <c r="K37" s="50">
         <f>200/1000</f>
         <v>0.2</v>
       </c>
-      <c r="L37" s="66">
+      <c r="L37" s="53">
+        <f t="shared" si="11"/>
+        <v>3.6222907107707401E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="45">
+        <v>3.78</v>
+      </c>
+      <c r="C38" s="3">
         <f t="shared" si="10"/>
-        <v>3.6222907107707401E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="53">
-        <v>3.78</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="9"/>
         <v>0.87711632608695655</v>
       </c>
-      <c r="D38" s="54">
+      <c r="D38" s="46">
         <v>0.125254</v>
       </c>
-      <c r="F38" s="59">
+      <c r="F38" s="48">
         <v>300</v>
       </c>
-      <c r="G38" s="63">
+      <c r="G38" s="50">
         <f>300/1000</f>
         <v>0.3</v>
       </c>
-      <c r="H38" s="49">
+      <c r="H38" s="42">
         <f>C67 + (F38 - B67) * ((C68 - C67) / (B68 - B67))</f>
         <v>10.45890106956522</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.8410135952059168</v>
       </c>
-      <c r="K38" s="63">
+      <c r="K38" s="50">
         <f>300/1000</f>
         <v>0.3</v>
       </c>
-      <c r="L38" s="66">
+      <c r="L38" s="53">
+        <f t="shared" si="11"/>
+        <v>8.330378258850303E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="45">
+        <v>4.46</v>
+      </c>
+      <c r="C39" s="3">
         <f t="shared" si="10"/>
-        <v>8.330378258850303E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="53">
-        <v>4.46</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="9"/>
         <v>1.0122908956521739</v>
       </c>
-      <c r="D39" s="54">
+      <c r="D39" s="46">
         <v>0.1351745695652174</v>
       </c>
-      <c r="F39" s="59">
+      <c r="F39" s="48">
         <v>400</v>
       </c>
-      <c r="G39" s="63">
+      <c r="G39" s="50">
         <v>0.4</v>
       </c>
-      <c r="H39" s="49">
+      <c r="H39" s="42">
         <f>C70 + (F39 - B70) * ((C71 - C70) / (B71 - B70))</f>
         <v>20.684617629353859</v>
       </c>
       <c r="I39" s="3">
+        <f t="shared" si="12"/>
+        <v>10.225716559788639</v>
+      </c>
+      <c r="K39" s="50">
+        <v>0.4</v>
+      </c>
+      <c r="L39" s="53">
         <f t="shared" si="11"/>
-        <v>10.225716559788639</v>
-      </c>
-      <c r="K39" s="63">
-        <v>0.4</v>
-      </c>
-      <c r="L39" s="66">
+        <v>4.6270210677776648E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="45">
+        <v>5.27</v>
+      </c>
+      <c r="C40" s="3">
         <f t="shared" si="10"/>
-        <v>4.6270210677776648E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="53">
-        <v>5.27</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="9"/>
         <v>1.1577564869565218</v>
       </c>
-      <c r="D40" s="54">
+      <c r="D40" s="46">
         <v>0.1454655913043478</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="48">
         <v>500</v>
       </c>
-      <c r="G40" s="63">
+      <c r="G40" s="50">
         <v>0.5</v>
       </c>
-      <c r="H40" s="49">
+      <c r="H40" s="42">
         <f>C71 + (F40 - B71) * ((C72 - C71) / (B72 - B71))</f>
         <v>39.802684974918094</v>
       </c>
@@ -8961,144 +8895,144 @@
         <f>H40-H39</f>
         <v>19.118067345564235</v>
       </c>
-      <c r="K40" s="63">
+      <c r="K40" s="50">
         <v>0.5</v>
       </c>
-      <c r="L40" s="66">
+      <c r="L40" s="53">
+        <f t="shared" si="11"/>
+        <v>8.650709206137662E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="45">
+        <v>6.21</v>
+      </c>
+      <c r="C41" s="3">
         <f t="shared" si="10"/>
-        <v>8.650709206137662E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="53">
-        <v>6.21</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="9"/>
         <v>1.3145914695652174</v>
       </c>
-      <c r="D41" s="54">
+      <c r="D41" s="46">
         <v>0.15683498260869566</v>
       </c>
-      <c r="F41" s="59">
+      <c r="F41" s="48">
         <v>630</v>
       </c>
-      <c r="G41" s="63">
+      <c r="G41" s="50">
         <v>0.63</v>
       </c>
-      <c r="H41" s="49">
+      <c r="H41" s="42">
         <f>C71 + (F41 - B71) * ((C72 - C71) / (B72 - B71))</f>
         <v>42.525445884979575</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" ref="I41:I43" si="12">H41-H40</f>
+        <f t="shared" ref="I41:I43" si="13">H41-H40</f>
         <v>2.7227609100614814</v>
       </c>
-      <c r="K41" s="63">
+      <c r="K41" s="50">
         <v>0.63</v>
       </c>
-      <c r="L41" s="66">
+      <c r="L41" s="53">
+        <f t="shared" si="11"/>
+        <v>1.2320185113400368E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="45">
+        <v>7.33</v>
+      </c>
+      <c r="C42" s="3">
         <f t="shared" si="10"/>
-        <v>1.2320185113400368E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="53">
-        <v>7.33</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="9"/>
         <v>1.4834078391304348</v>
       </c>
-      <c r="D42" s="54">
+      <c r="D42" s="46">
         <v>0.16881636956521742</v>
       </c>
-      <c r="F42" s="59">
+      <c r="F42" s="48">
         <v>700</v>
       </c>
-      <c r="G42" s="63">
+      <c r="G42" s="50">
         <v>0.7</v>
       </c>
-      <c r="H42" s="49">
+      <c r="H42" s="42">
         <f>C71 + (F42 - B71) * ((C72 - C71) / (B72 - B71))</f>
         <v>43.991547913474214</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4661020284946389</v>
       </c>
-      <c r="K42" s="63">
+      <c r="K42" s="50">
         <v>0.7</v>
       </c>
-      <c r="L42" s="66">
+      <c r="L42" s="53">
+        <f t="shared" si="11"/>
+        <v>6.6339458302924835E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="45">
+        <v>8.65</v>
+      </c>
+      <c r="C43" s="3">
         <f t="shared" si="10"/>
-        <v>6.6339458302924835E-4</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="53">
-        <v>8.65</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="9"/>
         <v>1.6652984695652175</v>
       </c>
-      <c r="D43" s="54">
+      <c r="D43" s="46">
         <v>0.18189063043478262</v>
       </c>
-      <c r="F43" s="59">
+      <c r="F43" s="48">
         <v>1000</v>
       </c>
-      <c r="G43" s="63">
+      <c r="G43" s="50">
         <v>1</v>
       </c>
-      <c r="H43" s="49">
+      <c r="H43" s="42">
         <f>C72 + (F43 - B72) * ((C73 - C72) / (B73 - B72))</f>
         <v>100.00000011739129</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>56.008452203917081</v>
       </c>
-      <c r="K43" s="63">
+      <c r="K43" s="50">
         <v>1</v>
       </c>
-      <c r="L43" s="66">
+      <c r="L43" s="53">
+        <f t="shared" si="11"/>
+        <v>2.5343191042496417E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="45">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="C44" s="3">
         <f t="shared" si="10"/>
-        <v>2.5343191042496417E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="53">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="9"/>
         <v>1.8639617782608697</v>
       </c>
-      <c r="D44" s="54">
+      <c r="D44" s="46">
         <v>0.19866330869565213</v>
       </c>
-      <c r="G44" s="58" t="s">
+      <c r="G44" s="47" t="s">
         <v>58</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L44" s="67">
+      <c r="L44" s="54">
         <f>SUM(L32:L43)</f>
         <v>4.5248868831398781E-2</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="53">
+      <c r="B45" s="45">
         <v>12.05</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.0826345956521739</v>
       </c>
-      <c r="D45" s="54">
+      <c r="D45" s="46">
         <v>0.21867281739130434</v>
       </c>
       <c r="L45" s="1" t="s">
@@ -9106,345 +9040,345 @@
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="53">
+      <c r="B46" s="45">
         <v>14.22</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.3316030086956521</v>
       </c>
-      <c r="D46" s="54">
+      <c r="D46" s="46">
         <v>0.24896841304347825</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="53">
+      <c r="B47" s="45">
         <v>16.78</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.6197704260869563</v>
       </c>
-      <c r="D47" s="54">
+      <c r="D47" s="46">
         <v>0.28816741739130436</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="53">
+      <c r="B48" s="45">
         <v>19.809999999999999</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.9570251782608694</v>
       </c>
-      <c r="D48" s="54">
+      <c r="D48" s="46">
         <v>0.33725475217391304</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="53">
+      <c r="B49" s="45">
         <v>23.37</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.1096920391304348</v>
       </c>
-      <c r="D49" s="54">
+      <c r="D49" s="46">
         <v>0.15266686086956519</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="53">
+      <c r="B50" s="45">
         <v>25</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.3513365173913043</v>
       </c>
-      <c r="D50" s="54">
+      <c r="D50" s="46">
         <v>0.24164447826086954</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="53">
+      <c r="B51" s="45">
         <v>27.58</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.8141872173913045</v>
       </c>
-      <c r="D51" s="54">
+      <c r="D51" s="46">
         <v>0.46285069999999995</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="53">
+      <c r="B52" s="45">
         <v>32.549999999999997</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.3410367260869567</v>
       </c>
-      <c r="D52" s="54">
+      <c r="D52" s="46">
         <v>0.52684950869565228</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="53">
+      <c r="B53" s="45">
         <v>38.409999999999997</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.920636043478261</v>
       </c>
-      <c r="D53" s="54">
+      <c r="D53" s="46">
         <v>0.57959931739130444</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="53">
+      <c r="B54" s="45">
         <v>45.32</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.5320725695652175</v>
       </c>
-      <c r="D54" s="54">
+      <c r="D54" s="46">
         <v>0.61143652608695653</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="53">
+      <c r="B55" s="45">
         <v>53.48</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.1275660913043479</v>
       </c>
-      <c r="D55" s="54">
+      <c r="D55" s="46">
         <v>0.5954935217391305</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="53">
+      <c r="B56" s="45">
         <v>63.11</v>
       </c>
       <c r="C56" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.6892284173913046</v>
       </c>
-      <c r="D56" s="54">
+      <c r="D56" s="46">
         <v>0.56166232608695643</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="53">
+      <c r="B57" s="45">
         <v>74.48</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.172364091304348</v>
       </c>
-      <c r="D57" s="54">
+      <c r="D57" s="46">
         <v>0.48313567391304357</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="53">
+      <c r="B58" s="45">
         <v>87.89</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.5740880043478267</v>
       </c>
-      <c r="D58" s="54">
+      <c r="D58" s="46">
         <v>0.40172391304347826</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="53">
+      <c r="B59" s="45">
         <v>103.72</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.8920909043478265</v>
       </c>
-      <c r="D59" s="54">
+      <c r="D59" s="46">
         <v>0.31800290000000003</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="53">
+      <c r="B60" s="45">
         <v>122.39</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.9221474608695654</v>
       </c>
-      <c r="D60" s="54">
+      <c r="D60" s="46">
         <v>3.0056556521739126E-2</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="53">
+      <c r="B61" s="45">
         <v>125</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.1459018260869573</v>
       </c>
-      <c r="D61" s="54">
+      <c r="D61" s="46">
         <v>0.22375436521739128</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="53">
+      <c r="B62" s="45">
         <v>144.43</v>
       </c>
       <c r="C62" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.3464342521739141</v>
       </c>
-      <c r="D62" s="54">
+      <c r="D62" s="46">
         <v>0.20053242608695654</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="53">
+      <c r="B63" s="45">
         <v>170.44</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.5040216608695669</v>
       </c>
-      <c r="D63" s="54">
+      <c r="D63" s="46">
         <v>0.15758740869565219</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="53">
+      <c r="B64" s="45">
         <v>201.13</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.6222402608695674</v>
       </c>
-      <c r="D64" s="54">
+      <c r="D64" s="46">
         <v>0.11821860000000001</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="53">
+      <c r="B65" s="45">
         <v>237.35</v>
       </c>
       <c r="C65" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.649954221739133</v>
       </c>
-      <c r="D65" s="54">
+      <c r="D65" s="46">
         <v>2.7713960869565214E-2</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="53">
+      <c r="B66" s="45">
         <v>250</v>
       </c>
       <c r="C66" s="3">
         <f>D66+C65</f>
         <v>8.7158762130434813</v>
       </c>
-      <c r="D66" s="54">
+      <c r="D66" s="46">
         <v>6.5921991304347824E-2</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="53">
+      <c r="B67" s="45">
         <v>280.08999999999997</v>
       </c>
       <c r="C67" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.7468423260869592</v>
       </c>
-      <c r="D67" s="54">
+      <c r="D67" s="46">
         <v>3.0966113043478259E-2</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="53">
+      <c r="B68" s="45">
         <v>300</v>
       </c>
       <c r="C68" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10.45890106956522</v>
       </c>
-      <c r="D68" s="54">
+      <c r="D68" s="46">
         <v>1.7120587434782608</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="53">
+      <c r="B69" s="45">
         <v>330.52</v>
       </c>
       <c r="C69" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.774185308695655</v>
       </c>
-      <c r="D69" s="54">
+      <c r="D69" s="46">
         <v>3.3152842391304347</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="53">
+      <c r="B70" s="45">
         <v>390.04</v>
       </c>
       <c r="C70" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17.662748386956522</v>
       </c>
-      <c r="D70" s="54">
+      <c r="D70" s="46">
         <v>3.8885630782608689</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="53">
+      <c r="B71" s="45">
         <v>460.27</v>
       </c>
       <c r="C71" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>38.970567352173916</v>
       </c>
-      <c r="D71" s="54">
+      <c r="D71" s="46">
         <v>21.30781896521739</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="53">
+      <c r="B72" s="45">
         <v>850</v>
       </c>
       <c r="C72" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.13319511739131</v>
       </c>
-      <c r="D72" s="54">
+      <c r="D72" s="46">
         <v>8.1626277652173904</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="53">
+      <c r="B73" s="45">
         <v>1000</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>100.00000011739129</v>
       </c>
-      <c r="D73" s="54">
+      <c r="D73" s="46">
         <v>52.866804999999992</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="60"/>
-      <c r="C74" s="61"/>
-      <c r="D74" s="62"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -9464,7 +9398,7 @@
   <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9477,18 +9411,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="79"/>
+      <c r="C2" s="66"/>
       <c r="H2" s="16" t="s">
         <v>14</v>
       </c>
@@ -9503,16 +9437,16 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="57" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="11">
@@ -9532,7 +9466,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12">
         <v>9.359555488395413E-3</v>
@@ -9855,12 +9789,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="22">
@@ -9912,7 +9846,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="23">
-        <f>I18/$I$29</f>
+        <f t="shared" ref="J18:J28" si="4">I18/$I$29</f>
         <v>2.8694404591104736E-3</v>
       </c>
       <c r="K18" s="23">
@@ -9942,7 +9876,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="23">
-        <f>I19/$I$29</f>
+        <f t="shared" si="4"/>
         <v>2.8694404591104736E-3</v>
       </c>
       <c r="K19" s="23">
@@ -9972,26 +9906,26 @@
         <v>3</v>
       </c>
       <c r="J20" s="23">
-        <f>I20/$I$29</f>
+        <f t="shared" si="4"/>
         <v>4.30416068866571E-3</v>
       </c>
       <c r="K20" s="23">
-        <f t="shared" ref="K20:K28" si="4">J20+K19</f>
+        <f t="shared" ref="K20:K28" si="5">J20+K19</f>
         <v>1.0043041606886658E-2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="80">
+      <c r="B21" s="9">
         <v>90</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="10">
         <v>0.15837104072398189</v>
       </c>
-      <c r="D21" s="81">
+      <c r="D21" s="10">
         <f t="shared" si="3"/>
         <v>0.89592760186307296</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21" s="1">
         <f t="shared" si="1"/>
         <v>159</v>
       </c>
@@ -10002,11 +9936,11 @@
         <v>4</v>
       </c>
       <c r="J21" s="23">
-        <f>I21/$I$29</f>
+        <f t="shared" si="4"/>
         <v>5.7388809182209472E-3</v>
       </c>
       <c r="K21" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5781922525107607E-2</v>
       </c>
     </row>
@@ -10032,19 +9966,19 @@
         <v>6</v>
       </c>
       <c r="J22" s="23">
-        <f>I22/$I$29</f>
+        <f t="shared" si="4"/>
         <v>8.60832137733142E-3</v>
       </c>
       <c r="K22" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4390243902439025E-2</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="57">
+      <c r="B23" s="8">
         <v>180</v>
       </c>
-      <c r="C23" s="81">
+      <c r="C23" s="10">
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="D23" s="10">
@@ -10062,11 +9996,11 @@
         <v>7</v>
       </c>
       <c r="J23" s="23">
-        <f>I23/$I$29</f>
+        <f t="shared" si="4"/>
         <v>1.0043041606886656E-2</v>
       </c>
       <c r="K23" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.443328550932568E-2</v>
       </c>
     </row>
@@ -10082,11 +10016,11 @@
         <v>46</v>
       </c>
       <c r="J24" s="23">
-        <f>I24/$I$29</f>
+        <f t="shared" si="4"/>
         <v>6.5997130559540887E-2</v>
       </c>
       <c r="K24" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.10043041606886657</v>
       </c>
     </row>
@@ -10098,11 +10032,11 @@
         <v>114</v>
       </c>
       <c r="J25" s="23">
-        <f>I25/$I$29</f>
+        <f t="shared" si="4"/>
         <v>0.16355810616929697</v>
       </c>
       <c r="K25" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.26398852223816355</v>
       </c>
     </row>
@@ -10121,11 +10055,11 @@
         <v>123</v>
       </c>
       <c r="J26" s="23">
-        <f>I26/$I$29</f>
+        <f t="shared" si="4"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="K26" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44045911047345765</v>
       </c>
     </row>
@@ -10144,11 +10078,11 @@
         <v>195</v>
       </c>
       <c r="J27" s="23">
-        <f>I27/$I$29</f>
+        <f t="shared" si="4"/>
         <v>0.27977044476327118</v>
       </c>
       <c r="K27" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.72022955523672882</v>
       </c>
     </row>
@@ -10167,11 +10101,11 @@
         <v>195</v>
       </c>
       <c r="J28" s="23">
-        <f>I28/$I$29</f>
+        <f t="shared" si="4"/>
         <v>0.27977044476327118</v>
       </c>
       <c r="K28" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10184,7 +10118,7 @@
         <v>697</v>
       </c>
       <c r="J29" s="17">
-        <f t="shared" ref="J29" si="5">SUM(J24:J28)</f>
+        <f t="shared" ref="J29" si="6">SUM(J24:J28)</f>
         <v>0.96556671449067433</v>
       </c>
     </row>
@@ -10285,10 +10219,10 @@
       <c r="F1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="41"/>
+      <c r="I1" s="69"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10317,11 +10251,11 @@
         <f>$I$20+($I$19-$I$20)*EXP(-14*A2)</f>
         <v>1.3290468742698638</v>
       </c>
-      <c r="H2" s="41" t="str">
+      <c r="H2" s="69" t="str">
         <f>B1</f>
         <v>Tri* (Dg/Ds = 10)</v>
       </c>
-      <c r="I2" s="41"/>
+      <c r="I2" s="69"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -10449,11 +10383,11 @@
         <f t="shared" si="4"/>
         <v>0.7870350317127095</v>
       </c>
-      <c r="H6" s="41" t="str">
+      <c r="H6" s="69" t="str">
         <f>C1</f>
         <v>Tri* (Dg/Ds = 20)</v>
       </c>
-      <c r="I6" s="41"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -10581,11 +10515,11 @@
         <f t="shared" si="4"/>
         <v>0.4774329545306662</v>
       </c>
-      <c r="H10" s="41" t="str">
+      <c r="H10" s="69" t="str">
         <f>D1</f>
         <v>Tri* (Dg/Ds = 35)</v>
       </c>
-      <c r="I10" s="41"/>
+      <c r="I10" s="69"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -10713,11 +10647,11 @@
         <f t="shared" si="4"/>
         <v>0.30058544185786273</v>
       </c>
-      <c r="H14" s="41" t="str">
+      <c r="H14" s="69" t="str">
         <f>E1</f>
         <v>Tri* (Dg/Ds = 50)</v>
       </c>
-      <c r="I14" s="41"/>
+      <c r="I14" s="69"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10842,11 +10776,11 @@
         <f t="shared" si="4"/>
         <v>0.1995685397000391</v>
       </c>
-      <c r="H18" s="41" t="str">
+      <c r="H18" s="69" t="str">
         <f>F1</f>
         <v>Tri* (Dg/Ds = 43.4)</v>
       </c>
-      <c r="I18" s="41"/>
+      <c r="I18" s="69"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -13152,13 +13086,13 @@
       <c r="B1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>

</xml_diff>

<commit_message>
wrapping some things up for MS V8
</commit_message>
<xml_diff>
--- a/data/bedload_tauc/Wilcock2002_tauc.xlsx
+++ b/data/bedload_tauc/Wilcock2002_tauc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data\bedload_tauc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6AD99E-FAF4-4A5C-A2C4-04C2A7A98145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3A2038-0735-4234-BFC2-003357074B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
   </bookViews>
   <sheets>
     <sheet name="Sand GSD calculations" sheetId="4" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Fs</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>Fines (&lt;0.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using Tri* = </t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,6 +714,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9397,7 +9403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529AA10A-7A72-482C-95E8-4CA51D7B8E74}">
   <dimension ref="B1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
@@ -13060,8 +13066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE20B856-AC4B-4A0B-8068-FF571A1CD20B}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13363,8 +13369,12 @@
       <c r="E16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>31</v>
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="71">
+        <f>B7</f>
+        <v>0.86746324999999902</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -14033,5 +14043,6 @@
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>